<commit_message>
table script minor tweaks
</commit_message>
<xml_diff>
--- a/VivelDialog.xlsx
+++ b/VivelDialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerja\Github\viveljs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A29F3E5-A7BF-4151-B4C0-31CDBD715611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7468AC9A-565B-4848-A0C7-A1921130768E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4716" uniqueCount="1307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4717" uniqueCount="1308">
   <si>
     <t>Segment</t>
   </si>
@@ -3445,9 +3445,6 @@
     <t>slides</t>
   </si>
   <si>
-    <t>audio/video</t>
-  </si>
-  <si>
     <t>rating</t>
   </si>
   <si>
@@ -3941,6 +3938,12 @@
   </si>
   <si>
     <t>190|190|190|190|190|190|190|190|190|190</t>
+  </si>
+  <si>
+    <t>Cinematic</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
@@ -4367,18 +4370,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4394,6 +4385,18 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4612,10 +4615,10 @@
   <dimension ref="A1:Z982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I516" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
+      <selection pane="bottomRight" activeCell="L526" sqref="L526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4637,37 +4640,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="73" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="73" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="73" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="74" t="s">
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="76"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="81"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -5502,7 +5505,7 @@
       <c r="M22" s="12"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
@@ -5510,7 +5513,7 @@
       <c r="S22" s="17"/>
       <c r="T22" s="19"/>
       <c r="U22" s="19" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
@@ -5780,7 +5783,7 @@
       <c r="K29" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="L29" s="77" t="s">
+      <c r="L29" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M29" s="12"/>
@@ -5788,10 +5791,10 @@
         <v>74</v>
       </c>
       <c r="O29" s="19" t="s">
+        <v>1145</v>
+      </c>
+      <c r="P29" s="19" t="s">
         <v>1146</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>1147</v>
       </c>
       <c r="Q29" s="19" t="s">
         <v>75</v>
@@ -5800,7 +5803,7 @@
       <c r="S29" s="17"/>
       <c r="T29" s="19"/>
       <c r="U29" s="19" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
@@ -5834,7 +5837,7 @@
       <c r="K30" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="L30" s="77" t="s">
+      <c r="L30" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M30" s="12"/>
@@ -5842,10 +5845,10 @@
         <v>79</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="P30" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q30" s="19" t="s">
         <v>80</v>
@@ -5854,7 +5857,7 @@
       <c r="S30" s="17"/>
       <c r="T30" s="19"/>
       <c r="U30" s="19" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
@@ -5888,7 +5891,7 @@
       <c r="K31" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="L31" s="77" t="s">
+      <c r="L31" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M31" s="12"/>
@@ -5896,10 +5899,10 @@
         <v>84</v>
       </c>
       <c r="O31" s="19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="P31" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q31" s="19" t="s">
         <v>85</v>
@@ -5908,7 +5911,7 @@
       <c r="S31" s="17"/>
       <c r="T31" s="19"/>
       <c r="U31" s="19" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
@@ -5942,7 +5945,7 @@
       <c r="K32" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="L32" s="77" t="s">
+      <c r="L32" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M32" s="12"/>
@@ -5950,10 +5953,10 @@
         <v>89</v>
       </c>
       <c r="O32" s="19" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="P32" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q32" s="19" t="s">
         <v>90</v>
@@ -5962,7 +5965,7 @@
       <c r="S32" s="17"/>
       <c r="T32" s="19"/>
       <c r="U32" s="19" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
@@ -5996,7 +5999,7 @@
       <c r="K33" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="L33" s="77" t="s">
+      <c r="L33" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M33" s="12"/>
@@ -6004,10 +6007,10 @@
         <v>94</v>
       </c>
       <c r="O33" s="19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="P33" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q33" s="23" t="s">
         <v>95</v>
@@ -6016,7 +6019,7 @@
       <c r="S33" s="17"/>
       <c r="T33" s="19"/>
       <c r="U33" s="19" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
@@ -6024,7 +6027,7 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="14"/>
       <c r="C34" s="20" t="s">
@@ -6050,7 +6053,7 @@
       <c r="K34" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="L34" s="77" t="s">
+      <c r="L34" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M34" s="12"/>
@@ -6058,10 +6061,10 @@
         <v>99</v>
       </c>
       <c r="O34" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="P34" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q34" s="19" t="s">
         <v>100</v>
@@ -6070,7 +6073,7 @@
       <c r="S34" s="17"/>
       <c r="T34" s="19"/>
       <c r="U34" s="19" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
@@ -6104,7 +6107,7 @@
       <c r="K35" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="L35" s="77" t="s">
+      <c r="L35" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M35" s="12"/>
@@ -6112,10 +6115,10 @@
         <v>104</v>
       </c>
       <c r="O35" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="P35" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q35" s="19" t="s">
         <v>105</v>
@@ -6124,7 +6127,7 @@
       <c r="S35" s="17"/>
       <c r="T35" s="19"/>
       <c r="U35" s="19" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
@@ -6158,7 +6161,7 @@
       <c r="K36" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="L36" s="77" t="s">
+      <c r="L36" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M36" s="12"/>
@@ -6166,10 +6169,10 @@
         <v>109</v>
       </c>
       <c r="O36" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="P36" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q36" s="19" t="s">
         <v>110</v>
@@ -6178,7 +6181,7 @@
       <c r="S36" s="17"/>
       <c r="T36" s="19"/>
       <c r="U36" s="19" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
@@ -6212,7 +6215,7 @@
       <c r="K37" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="L37" s="77" t="s">
+      <c r="L37" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M37" s="12"/>
@@ -6220,10 +6223,10 @@
         <v>114</v>
       </c>
       <c r="O37" s="19" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="P37" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q37" s="19" t="s">
         <v>115</v>
@@ -6232,7 +6235,7 @@
       <c r="S37" s="17"/>
       <c r="T37" s="19"/>
       <c r="U37" s="19" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
@@ -6266,7 +6269,7 @@
       <c r="K38" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="L38" s="77" t="s">
+      <c r="L38" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M38" s="12"/>
@@ -6274,10 +6277,10 @@
         <v>119</v>
       </c>
       <c r="O38" s="19" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="P38" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q38" s="19" t="s">
         <v>120</v>
@@ -6286,7 +6289,7 @@
       <c r="S38" s="17"/>
       <c r="T38" s="19"/>
       <c r="U38" s="19" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
@@ -6360,7 +6363,7 @@
       <c r="K40" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="L40" s="77" t="s">
+      <c r="L40" s="71" t="s">
         <v>1140</v>
       </c>
       <c r="M40" s="12"/>
@@ -6402,7 +6405,7 @@
       <c r="K41" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="L41" s="77" t="s">
+      <c r="L41" s="71" t="s">
         <v>1140</v>
       </c>
       <c r="M41" s="12"/>
@@ -6444,7 +6447,7 @@
       <c r="K42" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="L42" s="77" t="s">
+      <c r="L42" s="71" t="s">
         <v>1140</v>
       </c>
       <c r="M42" s="19"/>
@@ -6524,13 +6527,13 @@
       <c r="K44" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="L44" s="77" t="s">
+      <c r="L44" s="71" t="s">
         <v>1138</v>
       </c>
       <c r="M44" s="12"/>
       <c r="N44" s="19"/>
       <c r="O44" s="19" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
@@ -6756,13 +6759,13 @@
       <c r="K50" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="L50" s="77" t="s">
+      <c r="L50" s="71" t="s">
         <v>1138</v>
       </c>
       <c r="M50" s="12"/>
       <c r="N50" s="19"/>
       <c r="O50" s="19" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="P50" s="12"/>
       <c r="Q50" s="12"/>
@@ -6770,7 +6773,7 @@
       <c r="S50" s="17"/>
       <c r="T50" s="19"/>
       <c r="U50" s="19" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
@@ -6787,7 +6790,9 @@
       <c r="D51" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E51" s="12"/>
+      <c r="E51" s="12" t="s">
+        <v>1306</v>
+      </c>
       <c r="F51" s="12" t="s">
         <v>30</v>
       </c>
@@ -7110,7 +7115,7 @@
       <c r="K59" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="L59" s="77" t="s">
+      <c r="L59" s="71" t="s">
         <v>1138</v>
       </c>
       <c r="M59" s="12"/>
@@ -7404,13 +7409,13 @@
       <c r="K66" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="L66" s="78" t="s">
+      <c r="L66" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M66" s="25"/>
       <c r="N66" s="35"/>
       <c r="O66" s="35" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="P66" s="25"/>
       <c r="Q66" s="25"/>
@@ -7418,7 +7423,7 @@
       <c r="S66" s="17"/>
       <c r="T66" s="19"/>
       <c r="U66" s="19" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
@@ -7706,13 +7711,13 @@
       <c r="K73" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="L73" s="78" t="s">
+      <c r="L73" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M73" s="25"/>
       <c r="N73" s="35"/>
       <c r="O73" s="35" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="P73" s="25"/>
       <c r="Q73" s="25"/>
@@ -7720,7 +7725,7 @@
       <c r="S73" s="17"/>
       <c r="T73" s="37"/>
       <c r="U73" s="37" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
@@ -7754,13 +7759,13 @@
       <c r="K74" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="L74" s="78" t="s">
+      <c r="L74" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M74" s="25"/>
       <c r="N74" s="35"/>
       <c r="O74" s="35" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="P74" s="25"/>
       <c r="Q74" s="25"/>
@@ -7768,7 +7773,7 @@
       <c r="S74" s="17"/>
       <c r="T74" s="19"/>
       <c r="U74" s="19" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
@@ -7802,13 +7807,13 @@
       <c r="K75" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="L75" s="78" t="s">
+      <c r="L75" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M75" s="25"/>
       <c r="N75" s="35"/>
       <c r="O75" s="35" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="P75" s="25"/>
       <c r="Q75" s="25"/>
@@ -7816,7 +7821,7 @@
       <c r="S75" s="17"/>
       <c r="T75" s="19"/>
       <c r="U75" s="19" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
@@ -7926,13 +7931,13 @@
       <c r="K78" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="L78" s="79" t="s">
+      <c r="L78" s="73" t="s">
         <v>1138</v>
       </c>
       <c r="M78" s="27"/>
       <c r="N78" s="35"/>
       <c r="O78" s="35" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="P78" s="25"/>
       <c r="Q78" s="25"/>
@@ -8354,13 +8359,13 @@
       <c r="K89" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="L89" s="78" t="s">
+      <c r="L89" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M89" s="25"/>
       <c r="N89" s="35"/>
       <c r="O89" s="35" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="P89" s="25"/>
       <c r="Q89" s="25"/>
@@ -8396,13 +8401,13 @@
       <c r="K90" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="L90" s="78" t="s">
+      <c r="L90" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M90" s="25"/>
       <c r="N90" s="35"/>
       <c r="O90" s="35" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="P90" s="25"/>
       <c r="Q90" s="25"/>
@@ -8514,13 +8519,13 @@
       <c r="K93" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="L93" s="78" t="s">
+      <c r="L93" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M93" s="25"/>
       <c r="N93" s="35"/>
       <c r="O93" s="35" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="P93" s="25"/>
       <c r="Q93" s="25"/>
@@ -8528,7 +8533,7 @@
       <c r="S93" s="17"/>
       <c r="T93" s="19"/>
       <c r="U93" s="19" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
@@ -8910,13 +8915,13 @@
       <c r="K103" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="L103" s="78" t="s">
+      <c r="L103" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M103" s="25"/>
       <c r="N103" s="35"/>
       <c r="O103" s="35" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="P103" s="25"/>
       <c r="Q103" s="25"/>
@@ -9422,7 +9427,7 @@
       <c r="K116" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="L116" s="78" t="s">
+      <c r="L116" s="72" t="s">
         <v>1139</v>
       </c>
       <c r="M116" s="25"/>
@@ -9430,7 +9435,7 @@
         <v>258</v>
       </c>
       <c r="O116" s="35" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="P116" s="25"/>
       <c r="Q116" s="25"/>
@@ -9772,13 +9777,13 @@
       <c r="K125" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="L125" s="80" t="s">
+      <c r="L125" s="74" t="s">
         <v>1138</v>
       </c>
       <c r="M125" s="33"/>
       <c r="N125" s="35"/>
       <c r="O125" s="35" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="P125" s="25"/>
       <c r="Q125" s="25"/>
@@ -9786,7 +9791,7 @@
       <c r="S125" s="17"/>
       <c r="T125" s="19"/>
       <c r="U125" s="19" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="V125" s="1"/>
       <c r="W125" s="1"/>
@@ -10706,13 +10711,13 @@
       <c r="K149" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="L149" s="78" t="s">
+      <c r="L149" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M149" s="25"/>
       <c r="N149" s="35"/>
       <c r="O149" s="35" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="P149" s="25"/>
       <c r="Q149" s="25"/>
@@ -10942,13 +10947,13 @@
       <c r="K155" s="32" t="s">
         <v>307</v>
       </c>
-      <c r="L155" s="78" t="s">
+      <c r="L155" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M155" s="25"/>
       <c r="N155" s="35"/>
       <c r="O155" s="35" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="P155" s="25"/>
       <c r="Q155" s="25"/>
@@ -10956,7 +10961,7 @@
       <c r="S155" s="17"/>
       <c r="T155" s="19"/>
       <c r="U155" s="19" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
@@ -11258,16 +11263,16 @@
       <c r="K163" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="L163" s="78" t="s">
+      <c r="L163" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M163" s="25"/>
       <c r="N163" s="35"/>
       <c r="O163" s="35" t="s">
+        <v>1187</v>
+      </c>
+      <c r="P163" s="30" t="s">
         <v>1188</v>
-      </c>
-      <c r="P163" s="30" t="s">
-        <v>1189</v>
       </c>
       <c r="Q163" s="25" t="s">
         <v>320</v>
@@ -11418,13 +11423,13 @@
       <c r="K167" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="L167" s="78" t="s">
+      <c r="L167" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M167" s="25"/>
       <c r="N167" s="35"/>
       <c r="O167" s="35" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="P167" s="25"/>
       <c r="Q167" s="25"/>
@@ -11432,7 +11437,7 @@
       <c r="S167" s="17"/>
       <c r="T167" s="19"/>
       <c r="U167" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="V167" s="1"/>
       <c r="W167" s="1"/>
@@ -11784,13 +11789,13 @@
       <c r="K176" s="32" t="s">
         <v>343</v>
       </c>
-      <c r="L176" s="78" t="s">
+      <c r="L176" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M176" s="25"/>
       <c r="N176" s="35"/>
       <c r="O176" s="35" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="P176" s="25"/>
       <c r="Q176" s="25"/>
@@ -11800,7 +11805,7 @@
       </c>
       <c r="T176" s="19"/>
       <c r="U176" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="V176" s="1"/>
       <c r="W176" s="1"/>
@@ -11914,13 +11919,13 @@
       <c r="K179" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="L179" s="78" t="s">
+      <c r="L179" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M179" s="25"/>
       <c r="N179" s="35"/>
       <c r="O179" s="35" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="P179" s="25"/>
       <c r="Q179" s="25"/>
@@ -12034,13 +12039,13 @@
       <c r="K182" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="L182" s="78" t="s">
+      <c r="L182" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M182" s="48"/>
       <c r="N182" s="49"/>
       <c r="O182" s="50" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="P182" s="48"/>
       <c r="Q182" s="25"/>
@@ -12048,7 +12053,7 @@
       <c r="S182" s="17"/>
       <c r="T182" s="19"/>
       <c r="U182" s="19" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="V182" s="1"/>
       <c r="W182" s="1"/>
@@ -12202,7 +12207,7 @@
       <c r="K186" s="32" t="s">
         <v>362</v>
       </c>
-      <c r="L186" s="78" t="s">
+      <c r="L186" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M186" s="25"/>
@@ -12358,7 +12363,7 @@
       <c r="K190" s="32" t="s">
         <v>367</v>
       </c>
-      <c r="L190" s="78" t="s">
+      <c r="L190" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M190" s="25"/>
@@ -12668,13 +12673,13 @@
       <c r="K198" s="32" t="s">
         <v>377</v>
       </c>
-      <c r="L198" s="78" t="s">
+      <c r="L198" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M198" s="25"/>
       <c r="N198" s="35"/>
       <c r="O198" s="35" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="P198" s="25"/>
       <c r="Q198" s="25"/>
@@ -12682,7 +12687,7 @@
       <c r="S198" s="17"/>
       <c r="T198" s="19"/>
       <c r="U198" s="19" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="V198" s="1"/>
       <c r="W198" s="1"/>
@@ -12714,7 +12719,7 @@
       <c r="K199" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="L199" s="78" t="s">
+      <c r="L199" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M199" s="25"/>
@@ -12756,7 +12761,7 @@
       <c r="K200" s="32" t="s">
         <v>381</v>
       </c>
-      <c r="L200" s="78" t="s">
+      <c r="L200" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M200" s="25"/>
@@ -12836,7 +12841,7 @@
       <c r="K202" s="32" t="s">
         <v>384</v>
       </c>
-      <c r="L202" s="78" t="s">
+      <c r="L202" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M202" s="25"/>
@@ -12918,13 +12923,13 @@
       <c r="K204" s="32" t="s">
         <v>388</v>
       </c>
-      <c r="L204" s="78" t="s">
+      <c r="L204" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M204" s="25"/>
       <c r="N204" s="35"/>
       <c r="O204" s="35" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="P204" s="25"/>
       <c r="Q204" s="25"/>
@@ -12932,7 +12937,7 @@
       <c r="S204" s="17"/>
       <c r="T204" s="19"/>
       <c r="U204" s="19" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="V204" s="1"/>
       <c r="W204" s="1"/>
@@ -13042,13 +13047,13 @@
       <c r="K207" s="32" t="s">
         <v>393</v>
       </c>
-      <c r="L207" s="78" t="s">
+      <c r="L207" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M207" s="25"/>
       <c r="N207" s="35"/>
       <c r="O207" s="35" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="P207" s="25"/>
       <c r="Q207" s="25"/>
@@ -13056,7 +13061,7 @@
       <c r="S207" s="17"/>
       <c r="T207" s="19"/>
       <c r="U207" s="19" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="V207" s="1"/>
       <c r="W207" s="1"/>
@@ -13288,7 +13293,7 @@
       <c r="K213" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="L213" s="78" t="s">
+      <c r="L213" s="72" t="s">
         <v>1139</v>
       </c>
       <c r="M213" s="25"/>
@@ -13296,10 +13301,10 @@
         <v>405</v>
       </c>
       <c r="O213" s="35" t="s">
+        <v>1202</v>
+      </c>
+      <c r="P213" s="30" t="s">
         <v>1203</v>
-      </c>
-      <c r="P213" s="30" t="s">
-        <v>1204</v>
       </c>
       <c r="Q213" s="30" t="s">
         <v>406</v>
@@ -13310,7 +13315,7 @@
       <c r="S213" s="17"/>
       <c r="T213" s="19"/>
       <c r="U213" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="V213" s="1"/>
       <c r="W213" s="1"/>
@@ -13502,7 +13507,7 @@
       <c r="K218" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="L218" s="78" t="s">
+      <c r="L218" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M218" s="25"/>
@@ -13544,16 +13549,16 @@
       <c r="K219" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="L219" s="78" t="s">
+      <c r="L219" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M219" s="25"/>
       <c r="N219" s="35"/>
       <c r="O219" s="35" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="P219" s="30" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="Q219" s="25" t="s">
         <v>417</v>
@@ -13564,7 +13569,7 @@
       <c r="S219" s="52"/>
       <c r="T219" s="54"/>
       <c r="U219" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="V219" s="1"/>
       <c r="W219" s="1"/>
@@ -13756,7 +13761,7 @@
       <c r="K224" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="L224" s="78" t="s">
+      <c r="L224" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M224" s="25"/>
@@ -13798,16 +13803,16 @@
       <c r="K225" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="L225" s="78" t="s">
+      <c r="L225" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M225" s="25"/>
       <c r="N225" s="35"/>
       <c r="O225" s="35" t="s">
+        <v>1202</v>
+      </c>
+      <c r="P225" s="30" t="s">
         <v>1203</v>
-      </c>
-      <c r="P225" s="30" t="s">
-        <v>1204</v>
       </c>
       <c r="Q225" s="25" t="s">
         <v>424</v>
@@ -13818,7 +13823,7 @@
       <c r="S225" s="52"/>
       <c r="T225" s="54"/>
       <c r="U225" s="19" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="V225" s="1"/>
       <c r="W225" s="1"/>
@@ -14010,7 +14015,7 @@
       <c r="K230" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="L230" s="78" t="s">
+      <c r="L230" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M230" s="25"/>
@@ -14052,16 +14057,16 @@
       <c r="K231" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="L231" s="78" t="s">
+      <c r="L231" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M231" s="25"/>
       <c r="N231" s="35"/>
       <c r="O231" s="35" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="P231" s="30" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="Q231" s="25" t="s">
         <v>431</v>
@@ -14072,7 +14077,7 @@
       <c r="S231" s="52"/>
       <c r="T231" s="54"/>
       <c r="U231" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="V231" s="1"/>
       <c r="W231" s="1"/>
@@ -14264,7 +14269,7 @@
       <c r="K236" s="32" t="s">
         <v>437</v>
       </c>
-      <c r="L236" s="78" t="s">
+      <c r="L236" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M236" s="25"/>
@@ -14306,16 +14311,16 @@
       <c r="K237" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="L237" s="78" t="s">
+      <c r="L237" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M237" s="25"/>
       <c r="N237" s="35"/>
       <c r="O237" s="35" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="P237" s="30" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="Q237" s="25" t="s">
         <v>439</v>
@@ -14326,7 +14331,7 @@
       <c r="S237" s="52"/>
       <c r="T237" s="54"/>
       <c r="U237" s="19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="V237" s="1"/>
       <c r="W237" s="1"/>
@@ -14952,13 +14957,13 @@
       <c r="K253" s="32" t="s">
         <v>461</v>
       </c>
-      <c r="L253" s="78" t="s">
+      <c r="L253" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M253" s="25"/>
       <c r="N253" s="35"/>
       <c r="O253" s="35" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="P253" s="25"/>
       <c r="Q253" s="25"/>
@@ -14966,7 +14971,7 @@
       <c r="S253" s="52"/>
       <c r="T253" s="54"/>
       <c r="U253" s="19" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="V253" s="1"/>
       <c r="W253" s="1"/>
@@ -15272,13 +15277,13 @@
       <c r="K261" s="32" t="s">
         <v>472</v>
       </c>
-      <c r="L261" s="78" t="s">
+      <c r="L261" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M261" s="25"/>
       <c r="N261" s="35"/>
       <c r="O261" s="35" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="P261" s="25"/>
       <c r="Q261" s="25"/>
@@ -15440,13 +15445,13 @@
       <c r="K265" s="32" t="s">
         <v>480</v>
       </c>
-      <c r="L265" s="78" t="s">
+      <c r="L265" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M265" s="25"/>
       <c r="N265" s="35"/>
       <c r="O265" s="35" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="P265" s="25"/>
       <c r="Q265" s="25"/>
@@ -15560,13 +15565,13 @@
       <c r="K268" s="32" t="s">
         <v>485</v>
       </c>
-      <c r="L268" s="78" t="s">
+      <c r="L268" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M268" s="25"/>
       <c r="N268" s="35"/>
       <c r="O268" s="35" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="P268" s="25"/>
       <c r="Q268" s="25"/>
@@ -15678,13 +15683,13 @@
       <c r="K271" s="32" t="s">
         <v>488</v>
       </c>
-      <c r="L271" s="78" t="s">
+      <c r="L271" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M271" s="25"/>
       <c r="N271" s="35"/>
       <c r="O271" s="35" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="P271" s="25"/>
       <c r="Q271" s="25"/>
@@ -15692,7 +15697,7 @@
       <c r="S271" s="17"/>
       <c r="T271" s="19"/>
       <c r="U271" s="19" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="V271" s="1"/>
       <c r="W271" s="1"/>
@@ -15876,13 +15881,13 @@
       <c r="K276" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="L276" s="78" t="s">
+      <c r="L276" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M276" s="25"/>
       <c r="N276" s="35"/>
       <c r="O276" s="35" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="P276" s="25"/>
       <c r="Q276" s="25"/>
@@ -15890,7 +15895,7 @@
       <c r="S276" s="17"/>
       <c r="T276" s="19"/>
       <c r="U276" s="19" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="V276" s="1"/>
       <c r="W276" s="1"/>
@@ -16238,13 +16243,13 @@
       <c r="K285" s="32" t="s">
         <v>508</v>
       </c>
-      <c r="L285" s="78" t="s">
+      <c r="L285" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M285" s="25"/>
       <c r="N285" s="35"/>
       <c r="O285" s="35" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="P285" s="25"/>
       <c r="Q285" s="25"/>
@@ -16282,7 +16287,7 @@
       <c r="K286" s="32" t="s">
         <v>510</v>
       </c>
-      <c r="L286" s="78" t="s">
+      <c r="L286" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M286" s="25"/>
@@ -16326,13 +16331,13 @@
       <c r="K287" s="32" t="s">
         <v>512</v>
       </c>
-      <c r="L287" s="78" t="s">
+      <c r="L287" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M287" s="25"/>
       <c r="N287" s="35"/>
       <c r="O287" s="35" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="P287" s="25"/>
       <c r="Q287" s="25"/>
@@ -16340,7 +16345,7 @@
       <c r="S287" s="17"/>
       <c r="T287" s="19"/>
       <c r="U287" s="19" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="V287" s="1"/>
       <c r="W287" s="1"/>
@@ -16684,13 +16689,13 @@
       <c r="K296" s="32" t="s">
         <v>524</v>
       </c>
-      <c r="L296" s="78" t="s">
+      <c r="L296" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M296" s="25"/>
       <c r="N296" s="35"/>
       <c r="O296" s="35" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="P296" s="25"/>
       <c r="Q296" s="25"/>
@@ -16954,13 +16959,13 @@
       <c r="K303" s="32" t="s">
         <v>531</v>
       </c>
-      <c r="L303" s="78" t="s">
+      <c r="L303" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M303" s="25"/>
       <c r="N303" s="35"/>
       <c r="O303" s="35" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="P303" s="25"/>
       <c r="Q303" s="25"/>
@@ -17072,13 +17077,13 @@
       <c r="K306" s="32" t="s">
         <v>534</v>
       </c>
-      <c r="L306" s="78" t="s">
+      <c r="L306" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M306" s="25"/>
       <c r="N306" s="35"/>
       <c r="O306" s="35" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="P306" s="25"/>
       <c r="Q306" s="25"/>
@@ -17086,7 +17091,7 @@
       <c r="S306" s="17"/>
       <c r="T306" s="19"/>
       <c r="U306" s="19" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="V306" s="1"/>
       <c r="W306" s="1"/>
@@ -17194,13 +17199,13 @@
       <c r="K309" s="32" t="s">
         <v>538</v>
       </c>
-      <c r="L309" s="78" t="s">
+      <c r="L309" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M309" s="25"/>
       <c r="N309" s="35"/>
       <c r="O309" s="35" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="P309" s="25"/>
       <c r="Q309" s="25"/>
@@ -17208,7 +17213,7 @@
       <c r="S309" s="17"/>
       <c r="T309" s="19"/>
       <c r="U309" s="19" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="V309" s="1"/>
       <c r="W309" s="1"/>
@@ -17468,13 +17473,13 @@
       <c r="K316" s="32" t="s">
         <v>546</v>
       </c>
-      <c r="L316" s="78" t="s">
+      <c r="L316" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M316" s="25"/>
       <c r="N316" s="35"/>
       <c r="O316" s="35" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="P316" s="25"/>
       <c r="Q316" s="25"/>
@@ -17482,7 +17487,7 @@
       <c r="S316" s="17"/>
       <c r="T316" s="19"/>
       <c r="U316" s="19" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="V316" s="1"/>
       <c r="W316" s="1"/>
@@ -17590,13 +17595,13 @@
       <c r="K319" s="32" t="s">
         <v>550</v>
       </c>
-      <c r="L319" s="78" t="s">
+      <c r="L319" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M319" s="25"/>
       <c r="N319" s="35"/>
       <c r="O319" s="35" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="P319" s="25"/>
       <c r="Q319" s="25"/>
@@ -17604,7 +17609,7 @@
       <c r="S319" s="17"/>
       <c r="T319" s="19"/>
       <c r="U319" s="19" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="V319" s="1"/>
       <c r="W319" s="1"/>
@@ -17948,13 +17953,13 @@
       <c r="K328" s="32" t="s">
         <v>562</v>
       </c>
-      <c r="L328" s="78" t="s">
+      <c r="L328" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M328" s="25"/>
       <c r="N328" s="35"/>
       <c r="O328" s="35" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="P328" s="25"/>
       <c r="Q328" s="25"/>
@@ -17962,7 +17967,7 @@
       <c r="S328" s="17"/>
       <c r="T328" s="19"/>
       <c r="U328" s="19" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="V328" s="1"/>
       <c r="W328" s="1"/>
@@ -18032,13 +18037,13 @@
       <c r="K330" s="32" t="s">
         <v>562</v>
       </c>
-      <c r="L330" s="78" t="s">
+      <c r="L330" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M330" s="25"/>
       <c r="N330" s="35"/>
       <c r="O330" s="35" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="P330" s="25"/>
       <c r="Q330" s="25"/>
@@ -18046,7 +18051,7 @@
       <c r="S330" s="17"/>
       <c r="T330" s="19"/>
       <c r="U330" s="19" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="V330" s="1"/>
       <c r="W330" s="1"/>
@@ -18078,13 +18083,13 @@
       <c r="K331" s="32" t="s">
         <v>562</v>
       </c>
-      <c r="L331" s="78" t="s">
+      <c r="L331" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M331" s="25"/>
       <c r="N331" s="35"/>
       <c r="O331" s="35" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="P331" s="25"/>
       <c r="Q331" s="25"/>
@@ -18092,7 +18097,7 @@
       <c r="S331" s="17"/>
       <c r="T331" s="19"/>
       <c r="U331" s="19" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="V331" s="1"/>
       <c r="W331" s="1"/>
@@ -18162,7 +18167,7 @@
       <c r="K333" s="32" t="s">
         <v>566</v>
       </c>
-      <c r="L333" s="78" t="s">
+      <c r="L333" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M333" s="25"/>
@@ -18244,7 +18249,7 @@
       <c r="K335" s="32" t="s">
         <v>570</v>
       </c>
-      <c r="L335" s="78" t="s">
+      <c r="L335" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M335" s="25"/>
@@ -18440,7 +18445,7 @@
       <c r="K340" s="32" t="s">
         <v>577</v>
       </c>
-      <c r="L340" s="78" t="s">
+      <c r="L340" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M340" s="25"/>
@@ -18636,7 +18641,7 @@
       <c r="K345" s="32" t="s">
         <v>584</v>
       </c>
-      <c r="L345" s="78" t="s">
+      <c r="L345" s="72" t="s">
         <v>1139</v>
       </c>
       <c r="M345" s="25"/>
@@ -18644,10 +18649,10 @@
         <v>585</v>
       </c>
       <c r="O345" s="35" t="s">
+        <v>1238</v>
+      </c>
+      <c r="P345" s="30" t="s">
         <v>1239</v>
-      </c>
-      <c r="P345" s="30" t="s">
-        <v>1240</v>
       </c>
       <c r="Q345" s="25"/>
       <c r="R345" s="23" t="s">
@@ -18656,7 +18661,7 @@
       <c r="S345" s="17"/>
       <c r="T345" s="19"/>
       <c r="U345" s="19" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="V345" s="1"/>
       <c r="W345" s="1"/>
@@ -18764,7 +18769,7 @@
       <c r="K348" s="32" t="s">
         <v>590</v>
       </c>
-      <c r="L348" s="78" t="s">
+      <c r="L348" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M348" s="30"/>
@@ -19126,13 +19131,13 @@
       <c r="K357" s="32" t="s">
         <v>605</v>
       </c>
-      <c r="L357" s="78" t="s">
+      <c r="L357" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M357" s="25"/>
       <c r="N357" s="35"/>
       <c r="O357" s="35" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="P357" s="25"/>
       <c r="Q357" s="25"/>
@@ -19410,7 +19415,7 @@
       <c r="K364" s="32" t="s">
         <v>590</v>
       </c>
-      <c r="L364" s="78" t="s">
+      <c r="L364" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M364" s="30"/>
@@ -19812,13 +19817,13 @@
       <c r="K374" s="32" t="s">
         <v>605</v>
       </c>
-      <c r="L374" s="78" t="s">
+      <c r="L374" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M374" s="25"/>
       <c r="N374" s="35"/>
       <c r="O374" s="35" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="P374" s="25"/>
       <c r="Q374" s="25"/>
@@ -20294,7 +20299,7 @@
       <c r="K386" s="32" t="s">
         <v>590</v>
       </c>
-      <c r="L386" s="78" t="s">
+      <c r="L386" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M386" s="25"/>
@@ -21150,13 +21155,13 @@
       <c r="K408" s="32" t="s">
         <v>614</v>
       </c>
-      <c r="L408" s="78" t="s">
+      <c r="L408" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M408" s="25"/>
       <c r="N408" s="35"/>
       <c r="O408" s="35" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="P408" s="25"/>
       <c r="Q408" s="25"/>
@@ -22860,13 +22865,13 @@
       <c r="K452" s="32" t="s">
         <v>707</v>
       </c>
-      <c r="L452" s="78" t="s">
+      <c r="L452" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M452" s="25"/>
       <c r="N452" s="35"/>
       <c r="O452" s="35" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="P452" s="25"/>
       <c r="Q452" s="25"/>
@@ -22874,7 +22879,7 @@
       <c r="S452" s="17"/>
       <c r="T452" s="19"/>
       <c r="U452" s="19" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="V452" s="1"/>
       <c r="W452" s="1"/>
@@ -22944,13 +22949,13 @@
       <c r="K454" s="32" t="s">
         <v>710</v>
       </c>
-      <c r="L454" s="78" t="s">
+      <c r="L454" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M454" s="25"/>
       <c r="N454" s="35"/>
       <c r="O454" s="35" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="P454" s="25"/>
       <c r="Q454" s="25"/>
@@ -22958,7 +22963,7 @@
       <c r="S454" s="17"/>
       <c r="T454" s="19"/>
       <c r="U454" s="19" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="V454" s="1"/>
       <c r="W454" s="1"/>
@@ -23150,13 +23155,13 @@
       <c r="K459" s="32" t="s">
         <v>717</v>
       </c>
-      <c r="L459" s="78" t="s">
+      <c r="L459" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M459" s="25"/>
       <c r="N459" s="35"/>
       <c r="O459" s="35" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="P459" s="25"/>
       <c r="Q459" s="25"/>
@@ -23164,7 +23169,7 @@
       <c r="S459" s="17"/>
       <c r="T459" s="19"/>
       <c r="U459" s="19" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="V459" s="1"/>
       <c r="W459" s="1"/>
@@ -23394,13 +23399,13 @@
       <c r="K465" s="32" t="s">
         <v>724</v>
       </c>
-      <c r="L465" s="78" t="s">
+      <c r="L465" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M465" s="25"/>
       <c r="N465" s="35"/>
       <c r="O465" s="35" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="P465" s="25"/>
       <c r="Q465" s="25"/>
@@ -23408,7 +23413,7 @@
       <c r="S465" s="17"/>
       <c r="T465" s="19"/>
       <c r="U465" s="19" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="V465" s="1"/>
       <c r="W465" s="1"/>
@@ -23828,13 +23833,13 @@
       <c r="K476" s="32" t="s">
         <v>735</v>
       </c>
-      <c r="L476" s="78" t="s">
+      <c r="L476" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M476" s="25"/>
       <c r="N476" s="35"/>
       <c r="O476" s="35" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="P476" s="25"/>
       <c r="Q476" s="25"/>
@@ -23842,7 +23847,7 @@
       <c r="S476" s="17"/>
       <c r="T476" s="19"/>
       <c r="U476" s="19" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="V476" s="1"/>
       <c r="W476" s="1"/>
@@ -24108,7 +24113,7 @@
       <c r="K483" s="32" t="s">
         <v>746</v>
       </c>
-      <c r="L483" s="78" t="s">
+      <c r="L483" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M483" s="25"/>
@@ -24192,7 +24197,7 @@
       <c r="K485" s="32" t="s">
         <v>750</v>
       </c>
-      <c r="L485" s="78" t="s">
+      <c r="L485" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M485" s="25"/>
@@ -24848,13 +24853,13 @@
       <c r="K502" s="32" t="s">
         <v>770</v>
       </c>
-      <c r="L502" s="78" t="s">
+      <c r="L502" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M502" s="25"/>
       <c r="N502" s="35"/>
       <c r="O502" s="35" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="P502" s="25"/>
       <c r="Q502" s="25"/>
@@ -24862,7 +24867,7 @@
       <c r="S502" s="17"/>
       <c r="T502" s="19"/>
       <c r="U502" s="19" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="V502" s="1"/>
       <c r="W502" s="1"/>
@@ -24894,7 +24899,7 @@
       <c r="K503" s="32" t="s">
         <v>772</v>
       </c>
-      <c r="L503" s="78" t="s">
+      <c r="L503" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M503" s="25"/>
@@ -25208,13 +25213,13 @@
       <c r="K511" s="32" t="s">
         <v>782</v>
       </c>
-      <c r="L511" s="78" t="s">
+      <c r="L511" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M511" s="25"/>
       <c r="N511" s="35"/>
       <c r="O511" s="35" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="P511" s="25"/>
       <c r="Q511" s="25"/>
@@ -25222,7 +25227,7 @@
       <c r="S511" s="17"/>
       <c r="T511" s="19"/>
       <c r="U511" s="19" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="V511" s="1"/>
       <c r="W511" s="1"/>
@@ -25376,13 +25381,13 @@
       <c r="K515" s="32" t="s">
         <v>789</v>
       </c>
-      <c r="L515" s="78" t="s">
+      <c r="L515" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M515" s="25"/>
       <c r="N515" s="35"/>
       <c r="O515" s="35" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="P515" s="25"/>
       <c r="Q515" s="25"/>
@@ -25390,7 +25395,7 @@
       <c r="S515" s="17"/>
       <c r="T515" s="19"/>
       <c r="U515" s="19" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="V515" s="1"/>
       <c r="W515" s="1"/>
@@ -25540,13 +25545,13 @@
       <c r="K519" s="32" t="s">
         <v>795</v>
       </c>
-      <c r="L519" s="78" t="s">
+      <c r="L519" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M519" s="25"/>
       <c r="N519" s="35"/>
       <c r="O519" s="35" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="P519" s="25"/>
       <c r="Q519" s="25"/>
@@ -25554,7 +25559,7 @@
       <c r="S519" s="17"/>
       <c r="T519" s="19"/>
       <c r="U519" s="19" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="V519" s="1"/>
       <c r="W519" s="1"/>
@@ -25820,8 +25825,8 @@
       <c r="K526" s="32" t="s">
         <v>804</v>
       </c>
-      <c r="L526" s="78" t="s">
-        <v>1141</v>
+      <c r="L526" s="72" t="s">
+        <v>1307</v>
       </c>
       <c r="M526" s="25"/>
       <c r="N526" s="33"/>
@@ -25866,7 +25871,7 @@
       <c r="K527" s="32" t="s">
         <v>807</v>
       </c>
-      <c r="L527" s="78" t="s">
+      <c r="L527" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M527" s="30" t="s">
@@ -25874,10 +25879,10 @@
       </c>
       <c r="N527" s="35"/>
       <c r="O527" s="35" t="s">
+        <v>1261</v>
+      </c>
+      <c r="P527" s="30" t="s">
         <v>1262</v>
-      </c>
-      <c r="P527" s="30" t="s">
-        <v>1263</v>
       </c>
       <c r="Q527" s="25" t="s">
         <v>809</v>
@@ -25916,7 +25921,7 @@
       <c r="K528" s="32" t="s">
         <v>811</v>
       </c>
-      <c r="L528" s="78" t="s">
+      <c r="L528" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M528" s="30" t="s">
@@ -25924,10 +25929,10 @@
       </c>
       <c r="N528" s="35"/>
       <c r="O528" s="35" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="P528" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q528" s="25"/>
       <c r="R528" s="17"/>
@@ -25962,7 +25967,7 @@
       <c r="K529" s="32" t="s">
         <v>812</v>
       </c>
-      <c r="L529" s="78" t="s">
+      <c r="L529" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M529" s="30" t="s">
@@ -25970,10 +25975,10 @@
       </c>
       <c r="N529" s="35"/>
       <c r="O529" s="35" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="P529" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q529" s="25"/>
       <c r="R529" s="17"/>
@@ -26008,7 +26013,7 @@
       <c r="K530" s="32" t="s">
         <v>813</v>
       </c>
-      <c r="L530" s="78" t="s">
+      <c r="L530" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M530" s="30" t="s">
@@ -26016,10 +26021,10 @@
       </c>
       <c r="N530" s="35"/>
       <c r="O530" s="35" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="P530" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q530" s="25"/>
       <c r="R530" s="17"/>
@@ -26538,7 +26543,7 @@
       <c r="Y543" s="1"/>
       <c r="Z543" s="1"/>
     </row>
-    <row r="544" spans="1:26" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:26" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A544" s="25"/>
       <c r="B544" s="25"/>
       <c r="C544" s="25"/>
@@ -26560,16 +26565,16 @@
       <c r="K544" s="32" t="s">
         <v>831</v>
       </c>
-      <c r="L544" s="78" t="s">
+      <c r="L544" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M544" s="25"/>
       <c r="N544" s="35"/>
       <c r="O544" s="35" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="P544" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q544" s="25" t="s">
         <v>832</v>
@@ -26580,7 +26585,7 @@
       <c r="S544" s="17"/>
       <c r="T544" s="19"/>
       <c r="U544" s="19" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="V544" s="1"/>
       <c r="W544" s="1"/>
@@ -26848,16 +26853,16 @@
       <c r="K551" s="32" t="s">
         <v>843</v>
       </c>
-      <c r="L551" s="78" t="s">
+      <c r="L551" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M551" s="25"/>
       <c r="N551" s="35"/>
       <c r="O551" s="35" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="P551" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q551" s="25" t="s">
         <v>844</v>
@@ -26868,7 +26873,7 @@
       <c r="S551" s="17"/>
       <c r="T551" s="19"/>
       <c r="U551" s="19" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="V551" s="1"/>
       <c r="W551" s="1"/>
@@ -27686,8 +27691,8 @@
       <c r="K572" s="32" t="s">
         <v>873</v>
       </c>
-      <c r="L572" s="78" t="s">
-        <v>1141</v>
+      <c r="L572" s="72" t="s">
+        <v>1307</v>
       </c>
       <c r="M572" s="25"/>
       <c r="N572" s="33"/>
@@ -27730,7 +27735,7 @@
       <c r="K573" s="32" t="s">
         <v>876</v>
       </c>
-      <c r="L573" s="78" t="s">
+      <c r="L573" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M573" s="30" t="s">
@@ -27738,10 +27743,10 @@
       </c>
       <c r="N573" s="35"/>
       <c r="O573" s="35" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="P573" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q573" s="25" t="s">
         <v>878</v>
@@ -27780,7 +27785,7 @@
       <c r="K574" s="32" t="s">
         <v>811</v>
       </c>
-      <c r="L574" s="78" t="s">
+      <c r="L574" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M574" s="30" t="s">
@@ -27788,10 +27793,10 @@
       </c>
       <c r="N574" s="35"/>
       <c r="O574" s="35" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="P574" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q574" s="25"/>
       <c r="R574" s="17"/>
@@ -27804,7 +27809,7 @@
       <c r="Y574" s="1"/>
       <c r="Z574" s="1"/>
     </row>
-    <row r="575" spans="1:26" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:26" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A575" s="25"/>
       <c r="B575" s="25"/>
       <c r="C575" s="25"/>
@@ -27826,7 +27831,7 @@
       <c r="K575" s="32" t="s">
         <v>812</v>
       </c>
-      <c r="L575" s="78" t="s">
+      <c r="L575" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M575" s="30" t="s">
@@ -27834,10 +27839,10 @@
       </c>
       <c r="N575" s="35"/>
       <c r="O575" s="35" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="P575" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q575" s="25"/>
       <c r="R575" s="17"/>
@@ -27872,7 +27877,7 @@
       <c r="K576" s="32" t="s">
         <v>813</v>
       </c>
-      <c r="L576" s="78" t="s">
+      <c r="L576" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M576" s="30" t="s">
@@ -27880,10 +27885,10 @@
       </c>
       <c r="N576" s="35"/>
       <c r="O576" s="35" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="P576" s="30" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="Q576" s="25"/>
       <c r="R576" s="17"/>
@@ -28386,16 +28391,16 @@
       <c r="K589" s="32" t="s">
         <v>893</v>
       </c>
-      <c r="L589" s="78" t="s">
+      <c r="L589" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M589" s="25"/>
       <c r="N589" s="35"/>
       <c r="O589" s="35" t="s">
+        <v>1274</v>
+      </c>
+      <c r="P589" s="30" t="s">
         <v>1275</v>
-      </c>
-      <c r="P589" s="30" t="s">
-        <v>1276</v>
       </c>
       <c r="Q589" s="25" t="s">
         <v>894</v>
@@ -28406,7 +28411,7 @@
       <c r="S589" s="25"/>
       <c r="T589" s="35"/>
       <c r="U589" s="35" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="V589" s="1"/>
       <c r="W589" s="1"/>
@@ -28870,7 +28875,7 @@
       <c r="K601" s="32" t="s">
         <v>909</v>
       </c>
-      <c r="L601" s="78" t="s">
+      <c r="L601" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M601" s="25"/>
@@ -29634,13 +29639,13 @@
       <c r="K620" s="32" t="s">
         <v>937</v>
       </c>
-      <c r="L620" s="78" t="s">
+      <c r="L620" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M620" s="25"/>
       <c r="N620" s="35"/>
       <c r="O620" s="35" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="P620" s="25"/>
       <c r="Q620" s="25"/>
@@ -30022,13 +30027,13 @@
       <c r="K630" s="32" t="s">
         <v>948</v>
       </c>
-      <c r="L630" s="78" t="s">
+      <c r="L630" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M630" s="25"/>
       <c r="N630" s="35"/>
       <c r="O630" s="35" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="P630" s="25"/>
       <c r="Q630" s="25"/>
@@ -30998,7 +31003,7 @@
       <c r="K655" s="32" t="s">
         <v>975</v>
       </c>
-      <c r="L655" s="78" t="s">
+      <c r="L655" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M655" s="30"/>
@@ -31158,13 +31163,13 @@
       <c r="K659" s="32" t="s">
         <v>981</v>
       </c>
-      <c r="L659" s="78" t="s">
+      <c r="L659" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M659" s="25"/>
       <c r="N659" s="35"/>
       <c r="O659" s="35" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P659" s="25"/>
       <c r="Q659" s="25"/>
@@ -31172,7 +31177,7 @@
       <c r="S659" s="17"/>
       <c r="T659" s="19"/>
       <c r="U659" s="19" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="V659" s="1"/>
       <c r="W659" s="1"/>
@@ -31526,13 +31531,13 @@
       <c r="K668" s="32" t="s">
         <v>991</v>
       </c>
-      <c r="L668" s="78" t="s">
+      <c r="L668" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M668" s="25"/>
       <c r="N668" s="35"/>
       <c r="O668" s="35" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="P668" s="25"/>
       <c r="Q668" s="25"/>
@@ -31610,13 +31615,13 @@
       <c r="K670" s="32" t="s">
         <v>993</v>
       </c>
-      <c r="L670" s="78" t="s">
+      <c r="L670" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M670" s="25"/>
       <c r="N670" s="35"/>
       <c r="O670" s="35" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="P670" s="25"/>
       <c r="Q670" s="25"/>
@@ -31804,7 +31809,7 @@
       <c r="K675" s="32" t="s">
         <v>998</v>
       </c>
-      <c r="L675" s="78" t="s">
+      <c r="L675" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M675" s="30"/>
@@ -32766,7 +32771,7 @@
       <c r="K699" s="32" t="s">
         <v>556</v>
       </c>
-      <c r="L699" s="78" t="s">
+      <c r="L699" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M699" s="25"/>
@@ -32808,7 +32813,7 @@
       <c r="K700" s="32" t="s">
         <v>1026</v>
       </c>
-      <c r="L700" s="78" t="s">
+      <c r="L700" s="72" t="s">
         <v>1140</v>
       </c>
       <c r="M700" s="25"/>
@@ -33002,7 +33007,7 @@
       <c r="K705" s="32" t="s">
         <v>1031</v>
       </c>
-      <c r="L705" s="78" t="s">
+      <c r="L705" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M705" s="25"/>
@@ -33234,13 +33239,13 @@
       <c r="K711" s="32" t="s">
         <v>1038</v>
       </c>
-      <c r="L711" s="78" t="s">
+      <c r="L711" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M711" s="25"/>
       <c r="N711" s="35"/>
       <c r="O711" s="35" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="P711" s="25"/>
       <c r="Q711" s="25"/>
@@ -33400,13 +33405,13 @@
       <c r="K715" s="18" t="s">
         <v>1045</v>
       </c>
-      <c r="L715" s="81" t="s">
+      <c r="L715" s="75" t="s">
         <v>1138</v>
       </c>
       <c r="M715" s="16"/>
       <c r="N715" s="24"/>
       <c r="O715" s="24" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="P715" s="16"/>
       <c r="Q715" s="16"/>
@@ -33556,7 +33561,7 @@
       <c r="K719" s="18" t="s">
         <v>1049</v>
       </c>
-      <c r="L719" s="81" t="s">
+      <c r="L719" s="75" t="s">
         <v>1138</v>
       </c>
       <c r="M719" s="16"/>
@@ -33712,7 +33717,7 @@
       <c r="K723" s="18" t="s">
         <v>1054</v>
       </c>
-      <c r="L723" s="81" t="s">
+      <c r="L723" s="75" t="s">
         <v>1138</v>
       </c>
       <c r="M723" s="16"/>
@@ -33952,7 +33957,7 @@
       <c r="K729" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="L729" s="77" t="s">
+      <c r="L729" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M729" s="12"/>
@@ -33960,10 +33965,10 @@
         <v>74</v>
       </c>
       <c r="O729" s="19" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="P729" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q729" s="19" t="s">
         <v>1063</v>
@@ -33972,7 +33977,7 @@
       <c r="S729" s="17"/>
       <c r="T729" s="19"/>
       <c r="U729" s="19" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="V729" s="1"/>
       <c r="W729" s="1"/>
@@ -34006,7 +34011,7 @@
       <c r="K730" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="L730" s="77" t="s">
+      <c r="L730" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M730" s="12"/>
@@ -34014,10 +34019,10 @@
         <v>79</v>
       </c>
       <c r="O730" s="19" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="P730" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q730" s="19" t="s">
         <v>1066</v>
@@ -34026,7 +34031,7 @@
       <c r="S730" s="17"/>
       <c r="T730" s="19"/>
       <c r="U730" s="19" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="V730" s="1"/>
       <c r="W730" s="1"/>
@@ -34060,7 +34065,7 @@
       <c r="K731" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="L731" s="77" t="s">
+      <c r="L731" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M731" s="12"/>
@@ -34068,10 +34073,10 @@
         <v>84</v>
       </c>
       <c r="O731" s="19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="P731" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q731" s="19" t="s">
         <v>1069</v>
@@ -34080,7 +34085,7 @@
       <c r="S731" s="17"/>
       <c r="T731" s="19"/>
       <c r="U731" s="19" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="V731" s="1"/>
       <c r="W731" s="1"/>
@@ -34114,7 +34119,7 @@
       <c r="K732" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="L732" s="77" t="s">
+      <c r="L732" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M732" s="12"/>
@@ -34122,10 +34127,10 @@
         <v>89</v>
       </c>
       <c r="O732" s="19" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="P732" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q732" s="19" t="s">
         <v>1072</v>
@@ -34134,7 +34139,7 @@
       <c r="S732" s="17"/>
       <c r="T732" s="19"/>
       <c r="U732" s="19" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="V732" s="1"/>
       <c r="W732" s="1"/>
@@ -34168,7 +34173,7 @@
       <c r="K733" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="L733" s="77" t="s">
+      <c r="L733" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M733" s="12"/>
@@ -34176,10 +34181,10 @@
         <v>94</v>
       </c>
       <c r="O733" s="19" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="P733" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q733" s="23" t="s">
         <v>1075</v>
@@ -34188,7 +34193,7 @@
       <c r="S733" s="17"/>
       <c r="T733" s="19"/>
       <c r="U733" s="19" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="V733" s="1"/>
       <c r="W733" s="1"/>
@@ -34196,7 +34201,7 @@
       <c r="Y733" s="1"/>
       <c r="Z733" s="1"/>
     </row>
-    <row r="734" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="734" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A734" s="12"/>
       <c r="B734" s="14"/>
       <c r="C734" s="12" t="s">
@@ -34222,7 +34227,7 @@
       <c r="K734" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="L734" s="77" t="s">
+      <c r="L734" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M734" s="12"/>
@@ -34230,10 +34235,10 @@
         <v>99</v>
       </c>
       <c r="O734" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="P734" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q734" s="19" t="s">
         <v>1078</v>
@@ -34242,7 +34247,7 @@
       <c r="S734" s="17"/>
       <c r="T734" s="19"/>
       <c r="U734" s="19" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="V734" s="1"/>
       <c r="W734" s="1"/>
@@ -34276,7 +34281,7 @@
       <c r="K735" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="L735" s="77" t="s">
+      <c r="L735" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M735" s="12"/>
@@ -34284,10 +34289,10 @@
         <v>104</v>
       </c>
       <c r="O735" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="P735" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q735" s="19" t="s">
         <v>1081</v>
@@ -34296,7 +34301,7 @@
       <c r="S735" s="17"/>
       <c r="T735" s="19"/>
       <c r="U735" s="19" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="V735" s="1"/>
       <c r="W735" s="1"/>
@@ -34330,7 +34335,7 @@
       <c r="K736" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="L736" s="77" t="s">
+      <c r="L736" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M736" s="12"/>
@@ -34338,10 +34343,10 @@
         <v>109</v>
       </c>
       <c r="O736" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="P736" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q736" s="19" t="s">
         <v>1084</v>
@@ -34350,7 +34355,7 @@
       <c r="S736" s="17"/>
       <c r="T736" s="19"/>
       <c r="U736" s="19" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="V736" s="1"/>
       <c r="W736" s="1"/>
@@ -34384,7 +34389,7 @@
       <c r="K737" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="L737" s="77" t="s">
+      <c r="L737" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M737" s="12"/>
@@ -34392,10 +34397,10 @@
         <v>114</v>
       </c>
       <c r="O737" s="19" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="P737" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q737" s="19" t="s">
         <v>1087</v>
@@ -34404,7 +34409,7 @@
       <c r="S737" s="17"/>
       <c r="T737" s="19"/>
       <c r="U737" s="19" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="V737" s="1"/>
       <c r="W737" s="1"/>
@@ -34438,7 +34443,7 @@
       <c r="K738" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="L738" s="77" t="s">
+      <c r="L738" s="71" t="s">
         <v>1139</v>
       </c>
       <c r="M738" s="12"/>
@@ -34446,10 +34451,10 @@
         <v>119</v>
       </c>
       <c r="O738" s="19" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="P738" s="19" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Q738" s="19" t="s">
         <v>1090</v>
@@ -34458,7 +34463,7 @@
       <c r="S738" s="17"/>
       <c r="T738" s="19"/>
       <c r="U738" s="19" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="V738" s="1"/>
       <c r="W738" s="1"/>
@@ -34648,13 +34653,13 @@
       <c r="K743" s="32" t="s">
         <v>1098</v>
       </c>
-      <c r="L743" s="78" t="s">
-        <v>1142</v>
+      <c r="L743" s="72" t="s">
+        <v>1141</v>
       </c>
       <c r="M743" s="25"/>
       <c r="N743" s="35"/>
       <c r="O743" s="35" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="P743" s="25"/>
       <c r="Q743" s="25" t="s">
@@ -34664,7 +34669,7 @@
       <c r="S743" s="25"/>
       <c r="T743" s="35"/>
       <c r="U743" s="35" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="V743" s="1"/>
       <c r="W743" s="1"/>
@@ -34698,13 +34703,13 @@
       <c r="K744" s="32" t="s">
         <v>1102</v>
       </c>
-      <c r="L744" s="78" t="s">
-        <v>1142</v>
+      <c r="L744" s="72" t="s">
+        <v>1141</v>
       </c>
       <c r="M744" s="25"/>
       <c r="N744" s="35"/>
       <c r="O744" s="35" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="P744" s="25"/>
       <c r="Q744" s="25" t="s">
@@ -34714,7 +34719,7 @@
       <c r="S744" s="25"/>
       <c r="T744" s="35"/>
       <c r="U744" s="35" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="V744" s="1"/>
       <c r="W744" s="1"/>
@@ -34748,13 +34753,13 @@
       <c r="K745" s="32" t="s">
         <v>1106</v>
       </c>
-      <c r="L745" s="78" t="s">
-        <v>1142</v>
+      <c r="L745" s="72" t="s">
+        <v>1141</v>
       </c>
       <c r="M745" s="25"/>
       <c r="N745" s="35"/>
       <c r="O745" s="35" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="P745" s="25"/>
       <c r="Q745" s="25" t="s">
@@ -34764,7 +34769,7 @@
       <c r="S745" s="25"/>
       <c r="T745" s="35"/>
       <c r="U745" s="35" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="V745" s="1"/>
       <c r="W745" s="1"/>
@@ -34798,13 +34803,13 @@
       <c r="K746" s="32" t="s">
         <v>1110</v>
       </c>
-      <c r="L746" s="78" t="s">
-        <v>1142</v>
+      <c r="L746" s="72" t="s">
+        <v>1141</v>
       </c>
       <c r="M746" s="25"/>
       <c r="N746" s="35"/>
       <c r="O746" s="35" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="P746" s="25"/>
       <c r="Q746" s="25" t="s">
@@ -34814,7 +34819,7 @@
       <c r="S746" s="25"/>
       <c r="T746" s="35"/>
       <c r="U746" s="35" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="V746" s="1"/>
       <c r="W746" s="1"/>
@@ -34848,13 +34853,13 @@
       <c r="K747" s="32" t="s">
         <v>1115</v>
       </c>
-      <c r="L747" s="78" t="s">
+      <c r="L747" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="M747" s="25"/>
       <c r="N747" s="35"/>
       <c r="O747" s="35" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="P747" s="25"/>
       <c r="Q747" s="25" t="s">
@@ -34864,7 +34869,7 @@
       <c r="S747" s="25"/>
       <c r="T747" s="35"/>
       <c r="U747" s="35" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="V747" s="1"/>
       <c r="W747" s="1"/>
@@ -34898,8 +34903,8 @@
       <c r="K748" s="32" t="s">
         <v>1120</v>
       </c>
-      <c r="L748" s="78" t="s">
-        <v>1143</v>
+      <c r="L748" s="72" t="s">
+        <v>1142</v>
       </c>
       <c r="M748" s="25"/>
       <c r="N748" s="33"/>
@@ -34912,7 +34917,7 @@
       <c r="S748" s="25"/>
       <c r="T748" s="33"/>
       <c r="U748" s="35" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="V748" s="1"/>
       <c r="W748" s="1"/>
@@ -34946,13 +34951,13 @@
       <c r="K749" s="32" t="s">
         <v>1124</v>
       </c>
-      <c r="L749" s="78" t="s">
-        <v>1142</v>
+      <c r="L749" s="72" t="s">
+        <v>1141</v>
       </c>
       <c r="M749" s="25"/>
       <c r="N749" s="35"/>
       <c r="O749" s="35" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="P749" s="25"/>
       <c r="Q749" s="25" t="s">
@@ -34962,7 +34967,7 @@
       <c r="S749" s="25"/>
       <c r="T749" s="35"/>
       <c r="U749" s="35" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="V749" s="1"/>
       <c r="W749" s="1"/>
@@ -34996,13 +35001,13 @@
       <c r="K750" s="32" t="s">
         <v>1128</v>
       </c>
-      <c r="L750" s="78" t="s">
-        <v>1142</v>
+      <c r="L750" s="72" t="s">
+        <v>1141</v>
       </c>
       <c r="M750" s="25"/>
       <c r="N750" s="35"/>
       <c r="O750" s="35" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="P750" s="25"/>
       <c r="Q750" s="25" t="s">
@@ -35012,7 +35017,7 @@
       <c r="S750" s="25"/>
       <c r="T750" s="35"/>
       <c r="U750" s="35" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="V750" s="1"/>
       <c r="W750" s="1"/>
@@ -35046,8 +35051,8 @@
       <c r="K751" s="32" t="s">
         <v>1132</v>
       </c>
-      <c r="L751" s="78" t="s">
-        <v>1143</v>
+      <c r="L751" s="72" t="s">
+        <v>1142</v>
       </c>
       <c r="M751" s="25"/>
       <c r="N751" s="33"/>

</xml_diff>

<commit_message>
pra2-1 and pra2-4 changes
</commit_message>
<xml_diff>
--- a/VivelDialog.xlsx
+++ b/VivelDialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerja\Github\viveljs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421799EF-948B-4C26-8D09-85580761B597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971CA63-9489-4412-8554-32912EDA6939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2821,9 +2821,6 @@
     <t>Pelanggan berkali-kali melihat ke arah kasir.|Benda yang dicari pelanggan ada di kasir.|Pelanggan takut bertanya.</t>
   </si>
   <si>
-    <t>if pra2-1 true, go to 141, else go to 142</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
@@ -3034,9 +3031,6 @@
     <t>Pelanggan lebih memperhatikan kotak-kotak yang berukir.|Pelanggan suka benda-benda yang terlihat indah.|Benda yang dicari pelanggan memiliki harga yang mahal.</t>
   </si>
   <si>
-    <t>if pra2-4 true, go to 152, else go to 153</t>
-  </si>
-  <si>
     <t>152</t>
   </si>
   <si>
@@ -3914,6 +3908,12 @@
   </si>
   <si>
     <t>[ "var3", 1 ]</t>
+  </si>
+  <si>
+    <t>["pra2-1", true, 141]|["pra2-1", false, 142]</t>
+  </si>
+  <si>
+    <t>["pra2-4", true, 152]|["pra2-4", false, 153]</t>
   </si>
 </sst>
 </file>
@@ -4557,10 +4557,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="P566" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="T576" sqref="T576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4673,7 +4673,7 @@
         <v>21</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>22</v>
@@ -13255,7 +13255,7 @@
         <v>469</v>
       </c>
       <c r="R213" s="14" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="S213" s="14"/>
       <c r="T213" s="9"/>
@@ -13509,7 +13509,7 @@
         <v>481</v>
       </c>
       <c r="R219" s="14" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="S219" s="43"/>
       <c r="T219" s="44"/>
@@ -13763,7 +13763,7 @@
         <v>488</v>
       </c>
       <c r="R225" s="14" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="S225" s="43"/>
       <c r="T225" s="44"/>
@@ -14017,7 +14017,7 @@
         <v>495</v>
       </c>
       <c r="R231" s="14" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="S231" s="43"/>
       <c r="T231" s="44"/>
@@ -14271,7 +14271,7 @@
         <v>503</v>
       </c>
       <c r="R237" s="14" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="S237" s="43"/>
       <c r="T237" s="44"/>
@@ -18599,7 +18599,7 @@
       </c>
       <c r="Q345" s="19"/>
       <c r="R345" s="14" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="S345" s="14"/>
       <c r="T345" s="9"/>
@@ -25831,7 +25831,7 @@
         <v>926</v>
       </c>
       <c r="R527" s="14" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="S527" s="14"/>
       <c r="T527" s="9"/>
@@ -25972,10 +25972,10 @@
       <c r="Q530" s="19"/>
       <c r="R530" s="14"/>
       <c r="S530" s="14"/>
-      <c r="T530" s="9" t="s">
-        <v>933</v>
-      </c>
-      <c r="U530" s="9"/>
+      <c r="T530" s="9"/>
+      <c r="U530" s="9" t="s">
+        <v>1296</v>
+      </c>
       <c r="V530" s="1"/>
       <c r="W530" s="1"/>
       <c r="X530" s="1"/>
@@ -25986,7 +25986,7 @@
       <c r="A531" s="19"/>
       <c r="B531" s="19"/>
       <c r="C531" s="19" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D531" s="19"/>
       <c r="E531" s="22"/>
@@ -26004,7 +26004,7 @@
         <v>34</v>
       </c>
       <c r="K531" s="24" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="L531" s="19"/>
       <c r="M531" s="19"/>
@@ -26042,7 +26042,7 @@
         <v>34</v>
       </c>
       <c r="K532" s="24" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="L532" s="19"/>
       <c r="M532" s="19"/>
@@ -26080,7 +26080,7 @@
         <v>39</v>
       </c>
       <c r="K533" s="24" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="L533" s="19"/>
       <c r="M533" s="19"/>
@@ -26092,7 +26092,7 @@
       <c r="S533" s="14"/>
       <c r="T533" s="9"/>
       <c r="U533" s="9" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="V533" s="1"/>
       <c r="W533" s="1"/>
@@ -26104,7 +26104,7 @@
       <c r="A534" s="19"/>
       <c r="B534" s="19"/>
       <c r="C534" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D534" s="19"/>
       <c r="E534" s="22"/>
@@ -26122,7 +26122,7 @@
         <v>41</v>
       </c>
       <c r="K534" s="24" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="L534" s="19"/>
       <c r="M534" s="19"/>
@@ -26160,7 +26160,7 @@
         <v>41</v>
       </c>
       <c r="K535" s="24" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="L535" s="19"/>
       <c r="M535" s="19"/>
@@ -26198,7 +26198,7 @@
         <v>41</v>
       </c>
       <c r="K536" s="24" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="L536" s="19"/>
       <c r="M536" s="19"/>
@@ -26236,7 +26236,7 @@
         <v>41</v>
       </c>
       <c r="K537" s="24" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="L537" s="19"/>
       <c r="M537" s="19"/>
@@ -26274,7 +26274,7 @@
         <v>41</v>
       </c>
       <c r="K538" s="24" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="L538" s="19"/>
       <c r="M538" s="19"/>
@@ -26312,7 +26312,7 @@
         <v>41</v>
       </c>
       <c r="K539" s="24" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="L539" s="19"/>
       <c r="M539" s="19"/>
@@ -26350,7 +26350,7 @@
         <v>34</v>
       </c>
       <c r="K540" s="24" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="L540" s="19"/>
       <c r="M540" s="19"/>
@@ -26388,7 +26388,7 @@
         <v>41</v>
       </c>
       <c r="K541" s="24" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="L541" s="19"/>
       <c r="M541" s="19"/>
@@ -26400,7 +26400,7 @@
       <c r="S541" s="14"/>
       <c r="T541" s="9"/>
       <c r="U541" s="9" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="V541" s="1"/>
       <c r="W541" s="1"/>
@@ -26412,7 +26412,7 @@
       <c r="A542" s="19"/>
       <c r="B542" s="19"/>
       <c r="C542" s="19" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D542" s="19"/>
       <c r="E542" s="22"/>
@@ -26430,7 +26430,7 @@
         <v>39</v>
       </c>
       <c r="K542" s="24" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="L542" s="19"/>
       <c r="M542" s="19"/>
@@ -26468,7 +26468,7 @@
         <v>39</v>
       </c>
       <c r="K543" s="24" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="L543" s="19"/>
       <c r="M543" s="19"/>
@@ -26506,7 +26506,7 @@
         <v>41</v>
       </c>
       <c r="K544" s="24" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="L544" s="19" t="s">
         <v>60</v>
@@ -26514,21 +26514,21 @@
       <c r="M544" s="19"/>
       <c r="N544" s="25"/>
       <c r="O544" s="25" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="P544" s="19" t="s">
         <v>925</v>
       </c>
       <c r="Q544" s="19" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="R544" s="14" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="S544" s="14"/>
       <c r="T544" s="9"/>
       <c r="U544" s="9" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="V544" s="1"/>
       <c r="W544" s="1"/>
@@ -26540,7 +26540,7 @@
       <c r="A545" s="19"/>
       <c r="B545" s="19"/>
       <c r="C545" s="19" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D545" s="19"/>
       <c r="E545" s="22"/>
@@ -26558,7 +26558,7 @@
         <v>34</v>
       </c>
       <c r="K545" s="24" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="L545" s="19"/>
       <c r="M545" s="19"/>
@@ -26596,7 +26596,7 @@
         <v>34</v>
       </c>
       <c r="K546" s="24" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="L546" s="19"/>
       <c r="M546" s="19"/>
@@ -26608,7 +26608,7 @@
       <c r="S546" s="14"/>
       <c r="T546" s="9"/>
       <c r="U546" s="9" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="V546" s="1"/>
       <c r="W546" s="1"/>
@@ -26620,7 +26620,7 @@
       <c r="A547" s="19"/>
       <c r="B547" s="19"/>
       <c r="C547" s="19" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D547" s="19"/>
       <c r="E547" s="22"/>
@@ -26638,7 +26638,7 @@
         <v>41</v>
       </c>
       <c r="K547" s="24" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="L547" s="19"/>
       <c r="M547" s="19"/>
@@ -26676,7 +26676,7 @@
         <v>41</v>
       </c>
       <c r="K548" s="24" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="L548" s="19"/>
       <c r="M548" s="19"/>
@@ -26714,7 +26714,7 @@
         <v>34</v>
       </c>
       <c r="K549" s="24" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="L549" s="19"/>
       <c r="M549" s="19"/>
@@ -26752,7 +26752,7 @@
         <v>39</v>
       </c>
       <c r="K550" s="24" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="L550" s="19"/>
       <c r="M550" s="19"/>
@@ -26764,7 +26764,7 @@
       <c r="S550" s="14"/>
       <c r="T550" s="9"/>
       <c r="U550" s="9" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="V550" s="1"/>
       <c r="W550" s="1"/>
@@ -26776,7 +26776,7 @@
       <c r="A551" s="19"/>
       <c r="B551" s="19"/>
       <c r="C551" s="19" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D551" s="19"/>
       <c r="E551" s="22"/>
@@ -26794,7 +26794,7 @@
         <v>41</v>
       </c>
       <c r="K551" s="24" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="L551" s="19" t="s">
         <v>60</v>
@@ -26802,21 +26802,21 @@
       <c r="M551" s="19"/>
       <c r="N551" s="25"/>
       <c r="O551" s="25" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="P551" s="19" t="s">
         <v>925</v>
       </c>
       <c r="Q551" s="19" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="R551" s="14" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="S551" s="14"/>
       <c r="T551" s="9"/>
       <c r="U551" s="9" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="V551" s="1"/>
       <c r="W551" s="1"/>
@@ -26828,7 +26828,7 @@
       <c r="A552" s="19"/>
       <c r="B552" s="19"/>
       <c r="C552" s="19" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D552" s="19"/>
       <c r="E552" s="22"/>
@@ -26846,7 +26846,7 @@
         <v>34</v>
       </c>
       <c r="K552" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="L552" s="19"/>
       <c r="M552" s="19"/>
@@ -26884,7 +26884,7 @@
         <v>34</v>
       </c>
       <c r="K553" s="24" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="L553" s="19"/>
       <c r="M553" s="19"/>
@@ -26896,7 +26896,7 @@
       <c r="S553" s="14"/>
       <c r="T553" s="9"/>
       <c r="U553" s="9" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V553" s="1"/>
       <c r="W553" s="1"/>
@@ -26908,7 +26908,7 @@
       <c r="A554" s="19"/>
       <c r="B554" s="19"/>
       <c r="C554" s="19" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D554" s="19"/>
       <c r="E554" s="22"/>
@@ -26926,7 +26926,7 @@
         <v>41</v>
       </c>
       <c r="K554" s="24" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="L554" s="19"/>
       <c r="M554" s="19"/>
@@ -26964,7 +26964,7 @@
         <v>41</v>
       </c>
       <c r="K555" s="24" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="L555" s="19"/>
       <c r="M555" s="19"/>
@@ -27002,7 +27002,7 @@
         <v>39</v>
       </c>
       <c r="K556" s="24" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="L556" s="19"/>
       <c r="M556" s="19"/>
@@ -27040,7 +27040,7 @@
         <v>41</v>
       </c>
       <c r="K557" s="24" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="L557" s="19"/>
       <c r="M557" s="19"/>
@@ -27078,7 +27078,7 @@
         <v>39</v>
       </c>
       <c r="K558" s="24" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="L558" s="19"/>
       <c r="M558" s="19"/>
@@ -27090,7 +27090,7 @@
       <c r="S558" s="14"/>
       <c r="T558" s="25"/>
       <c r="U558" s="25" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V558" s="1"/>
       <c r="W558" s="1"/>
@@ -27102,7 +27102,7 @@
       <c r="A559" s="19"/>
       <c r="B559" s="19"/>
       <c r="C559" s="19" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D559" s="19"/>
       <c r="E559" s="22"/>
@@ -27120,7 +27120,7 @@
         <v>39</v>
       </c>
       <c r="K559" s="24" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="L559" s="19"/>
       <c r="M559" s="19"/>
@@ -27158,7 +27158,7 @@
         <v>39</v>
       </c>
       <c r="K560" s="24" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="L560" s="19"/>
       <c r="M560" s="19"/>
@@ -27191,16 +27191,16 @@
         <v>595</v>
       </c>
       <c r="H561" s="23" t="s">
+        <v>978</v>
+      </c>
+      <c r="I561" s="19" t="s">
         <v>979</v>
-      </c>
-      <c r="I561" s="19" t="s">
-        <v>980</v>
       </c>
       <c r="J561" s="23" t="s">
         <v>54</v>
       </c>
       <c r="K561" s="24" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L561" s="19"/>
       <c r="M561" s="19"/>
@@ -27238,7 +27238,7 @@
         <v>39</v>
       </c>
       <c r="K562" s="24" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="L562" s="19"/>
       <c r="M562" s="19"/>
@@ -27269,16 +27269,16 @@
         <v>595</v>
       </c>
       <c r="H563" s="23" t="s">
+        <v>978</v>
+      </c>
+      <c r="I563" s="19" t="s">
         <v>979</v>
-      </c>
-      <c r="I563" s="19" t="s">
-        <v>980</v>
       </c>
       <c r="J563" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K563" s="24" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="L563" s="19"/>
       <c r="M563" s="19"/>
@@ -27316,7 +27316,7 @@
         <v>34</v>
       </c>
       <c r="K564" s="24" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="L564" s="19"/>
       <c r="M564" s="19"/>
@@ -27347,16 +27347,16 @@
         <v>595</v>
       </c>
       <c r="H565" s="23" t="s">
+        <v>978</v>
+      </c>
+      <c r="I565" s="19" t="s">
         <v>979</v>
-      </c>
-      <c r="I565" s="19" t="s">
-        <v>980</v>
       </c>
       <c r="J565" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K565" s="24" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="L565" s="19"/>
       <c r="M565" s="19"/>
@@ -27394,7 +27394,7 @@
         <v>34</v>
       </c>
       <c r="K566" s="24" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="L566" s="19"/>
       <c r="M566" s="19"/>
@@ -27434,7 +27434,7 @@
         <v>34</v>
       </c>
       <c r="K567" s="24" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="L567" s="19"/>
       <c r="M567" s="19"/>
@@ -27472,7 +27472,7 @@
         <v>34</v>
       </c>
       <c r="K568" s="24" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="L568" s="19"/>
       <c r="M568" s="19"/>
@@ -27510,7 +27510,7 @@
         <v>39</v>
       </c>
       <c r="K569" s="24" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="L569" s="19"/>
       <c r="M569" s="19"/>
@@ -27548,7 +27548,7 @@
         <v>39</v>
       </c>
       <c r="K570" s="24" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="L570" s="19"/>
       <c r="M570" s="19"/>
@@ -27586,7 +27586,7 @@
         <v>34</v>
       </c>
       <c r="K571" s="24" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="L571" s="19"/>
       <c r="M571" s="19"/>
@@ -27600,7 +27600,7 @@
       </c>
       <c r="T571" s="25"/>
       <c r="U571" s="25" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="V571" s="1"/>
       <c r="W571" s="1"/>
@@ -27612,10 +27612,10 @@
       <c r="A572" s="19"/>
       <c r="B572" s="19"/>
       <c r="C572" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="D572" s="19" t="s">
         <v>992</v>
-      </c>
-      <c r="D572" s="19" t="s">
-        <v>993</v>
       </c>
       <c r="E572" s="22"/>
       <c r="F572" s="22" t="s">
@@ -27632,7 +27632,7 @@
         <v>39</v>
       </c>
       <c r="K572" s="24" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="L572" s="19" t="s">
         <v>919</v>
@@ -27640,7 +27640,7 @@
       <c r="M572" s="19"/>
       <c r="N572" s="25"/>
       <c r="O572" s="25" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P572" s="19"/>
       <c r="Q572" s="19"/>
@@ -27658,7 +27658,7 @@
       <c r="A573" s="19"/>
       <c r="B573" s="19"/>
       <c r="C573" s="19" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D573" s="19"/>
       <c r="E573" s="22"/>
@@ -27676,26 +27676,26 @@
         <v>41</v>
       </c>
       <c r="K573" s="24" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="L573" s="19" t="s">
         <v>60</v>
       </c>
       <c r="M573" s="19" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="N573" s="25"/>
       <c r="O573" s="25" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P573" s="19" t="s">
         <v>925</v>
       </c>
       <c r="Q573" s="19" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="R573" s="14" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="S573" s="14"/>
       <c r="T573" s="25"/>
@@ -27732,11 +27732,11 @@
         <v>60</v>
       </c>
       <c r="M574" s="19" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="N574" s="25"/>
       <c r="O574" s="25" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P574" s="19" t="s">
         <v>925</v>
@@ -27778,11 +27778,11 @@
         <v>60</v>
       </c>
       <c r="M575" s="19" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="N575" s="25"/>
       <c r="O575" s="25" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P575" s="19" t="s">
         <v>925</v>
@@ -27824,11 +27824,11 @@
         <v>60</v>
       </c>
       <c r="M576" s="19" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="N576" s="25"/>
       <c r="O576" s="25" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="P576" s="19" t="s">
         <v>925</v>
@@ -27836,10 +27836,10 @@
       <c r="Q576" s="19"/>
       <c r="R576" s="14"/>
       <c r="S576" s="14"/>
-      <c r="T576" s="25" t="s">
-        <v>1004</v>
-      </c>
-      <c r="U576" s="25"/>
+      <c r="T576" s="25"/>
+      <c r="U576" s="25" t="s">
+        <v>1297</v>
+      </c>
       <c r="V576" s="1"/>
       <c r="W576" s="1"/>
       <c r="X576" s="1"/>
@@ -27850,7 +27850,7 @@
       <c r="A577" s="19"/>
       <c r="B577" s="19"/>
       <c r="C577" s="19" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="D577" s="19"/>
       <c r="E577" s="22"/>
@@ -27868,7 +27868,7 @@
         <v>34</v>
       </c>
       <c r="K577" s="24" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="L577" s="19"/>
       <c r="M577" s="19"/>
@@ -27906,7 +27906,7 @@
         <v>34</v>
       </c>
       <c r="K578" s="24" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L578" s="19"/>
       <c r="M578" s="19"/>
@@ -27944,7 +27944,7 @@
         <v>34</v>
       </c>
       <c r="K579" s="24" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="L579" s="19"/>
       <c r="M579" s="19"/>
@@ -27956,7 +27956,7 @@
       <c r="S579" s="14"/>
       <c r="T579" s="25"/>
       <c r="U579" s="25" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="V579" s="1"/>
       <c r="W579" s="1"/>
@@ -27968,7 +27968,7 @@
       <c r="A580" s="19"/>
       <c r="B580" s="19"/>
       <c r="C580" s="19" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D580" s="19"/>
       <c r="E580" s="22"/>
@@ -27986,7 +27986,7 @@
         <v>41</v>
       </c>
       <c r="K580" s="24" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="L580" s="19"/>
       <c r="M580" s="19"/>
@@ -28024,7 +28024,7 @@
         <v>41</v>
       </c>
       <c r="K581" s="24" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="L581" s="19"/>
       <c r="M581" s="19"/>
@@ -28062,7 +28062,7 @@
         <v>41</v>
       </c>
       <c r="K582" s="24" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="L582" s="19"/>
       <c r="M582" s="19"/>
@@ -28100,7 +28100,7 @@
         <v>41</v>
       </c>
       <c r="K583" s="24" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="L583" s="19"/>
       <c r="M583" s="19"/>
@@ -28138,7 +28138,7 @@
         <v>41</v>
       </c>
       <c r="K584" s="24" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="L584" s="19"/>
       <c r="M584" s="19"/>
@@ -28176,7 +28176,7 @@
         <v>41</v>
       </c>
       <c r="K585" s="24" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="L585" s="19"/>
       <c r="M585" s="19"/>
@@ -28214,7 +28214,7 @@
         <v>34</v>
       </c>
       <c r="K586" s="24" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="L586" s="19"/>
       <c r="M586" s="19"/>
@@ -28252,7 +28252,7 @@
         <v>39</v>
       </c>
       <c r="K587" s="24" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="L587" s="19"/>
       <c r="M587" s="19"/>
@@ -28264,7 +28264,7 @@
       <c r="S587" s="19"/>
       <c r="T587" s="25"/>
       <c r="U587" s="25" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="V587" s="1"/>
       <c r="W587" s="1"/>
@@ -28276,7 +28276,7 @@
       <c r="A588" s="19"/>
       <c r="B588" s="19"/>
       <c r="C588" s="19" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="D588" s="19"/>
       <c r="E588" s="22"/>
@@ -28294,7 +28294,7 @@
         <v>41</v>
       </c>
       <c r="K588" s="24" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="L588" s="19"/>
       <c r="M588" s="19"/>
@@ -28332,7 +28332,7 @@
         <v>41</v>
       </c>
       <c r="K589" s="24" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="L589" s="19" t="s">
         <v>60</v>
@@ -28340,21 +28340,21 @@
       <c r="M589" s="19"/>
       <c r="N589" s="25"/>
       <c r="O589" s="25" t="s">
+        <v>1016</v>
+      </c>
+      <c r="P589" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="Q589" s="19" t="s">
         <v>1018</v>
       </c>
-      <c r="P589" s="19" t="s">
-        <v>1019</v>
-      </c>
-      <c r="Q589" s="19" t="s">
-        <v>1020</v>
-      </c>
       <c r="R589" s="19" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="S589" s="19"/>
       <c r="T589" s="25"/>
       <c r="U589" s="25" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="V589" s="1"/>
       <c r="W589" s="1"/>
@@ -28366,7 +28366,7 @@
       <c r="A590" s="19"/>
       <c r="B590" s="19"/>
       <c r="C590" s="19" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="D590" s="19"/>
       <c r="E590" s="22"/>
@@ -28384,7 +28384,7 @@
         <v>34</v>
       </c>
       <c r="K590" s="24" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="L590" s="19"/>
       <c r="M590" s="19"/>
@@ -28422,7 +28422,7 @@
         <v>34</v>
       </c>
       <c r="K591" s="24" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="L591" s="19"/>
       <c r="M591" s="19"/>
@@ -28434,7 +28434,7 @@
       <c r="S591" s="19"/>
       <c r="T591" s="25"/>
       <c r="U591" s="25" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="V591" s="1"/>
       <c r="W591" s="1"/>
@@ -28446,7 +28446,7 @@
       <c r="A592" s="19"/>
       <c r="B592" s="19"/>
       <c r="C592" s="19" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="D592" s="19"/>
       <c r="E592" s="22"/>
@@ -28464,7 +28464,7 @@
         <v>41</v>
       </c>
       <c r="K592" s="24" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="L592" s="19"/>
       <c r="M592" s="19"/>
@@ -28502,7 +28502,7 @@
         <v>41</v>
       </c>
       <c r="K593" s="24" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="L593" s="19"/>
       <c r="M593" s="19"/>
@@ -28540,7 +28540,7 @@
         <v>34</v>
       </c>
       <c r="K594" s="24" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="L594" s="19"/>
       <c r="M594" s="19"/>
@@ -28578,7 +28578,7 @@
         <v>39</v>
       </c>
       <c r="K595" s="24" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="L595" s="19"/>
       <c r="M595" s="19"/>
@@ -28590,7 +28590,7 @@
       <c r="S595" s="19"/>
       <c r="T595" s="25"/>
       <c r="U595" s="25" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="V595" s="1"/>
       <c r="W595" s="1"/>
@@ -28602,7 +28602,7 @@
       <c r="A596" s="19"/>
       <c r="B596" s="19"/>
       <c r="C596" s="19" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D596" s="19"/>
       <c r="E596" s="22"/>
@@ -28620,7 +28620,7 @@
         <v>39</v>
       </c>
       <c r="K596" s="24" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="L596" s="19"/>
       <c r="M596" s="19"/>
@@ -28658,7 +28658,7 @@
         <v>39</v>
       </c>
       <c r="K597" s="24" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="L597" s="19"/>
       <c r="M597" s="19"/>
@@ -28691,16 +28691,16 @@
         <v>595</v>
       </c>
       <c r="H598" s="23" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I598" s="19" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J598" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K598" s="24" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="L598" s="19"/>
       <c r="M598" s="19"/>
@@ -28738,7 +28738,7 @@
         <v>39</v>
       </c>
       <c r="K599" s="24" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="L599" s="19"/>
       <c r="M599" s="19"/>
@@ -28769,16 +28769,16 @@
         <v>595</v>
       </c>
       <c r="H600" s="23" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I600" s="19" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J600" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K600" s="24" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="L600" s="19"/>
       <c r="M600" s="19"/>
@@ -28816,14 +28816,14 @@
         <v>39</v>
       </c>
       <c r="K601" s="24" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="L601" s="19" t="s">
         <v>149</v>
       </c>
       <c r="M601" s="19"/>
       <c r="N601" s="25" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="O601" s="25"/>
       <c r="P601" s="19"/>
@@ -28851,16 +28851,16 @@
         <v>595</v>
       </c>
       <c r="H602" s="23" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I602" s="19" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J602" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K602" s="24" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="L602" s="19"/>
       <c r="M602" s="19"/>
@@ -28898,7 +28898,7 @@
         <v>34</v>
       </c>
       <c r="K603" s="24" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="L603" s="19"/>
       <c r="M603" s="19"/>
@@ -28929,16 +28929,16 @@
         <v>595</v>
       </c>
       <c r="H604" s="23" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I604" s="19" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J604" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K604" s="24" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="L604" s="19"/>
       <c r="M604" s="19"/>
@@ -28969,16 +28969,16 @@
         <v>595</v>
       </c>
       <c r="H605" s="23" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I605" s="19" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J605" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K605" s="24" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="L605" s="19"/>
       <c r="M605" s="19"/>
@@ -29016,7 +29016,7 @@
         <v>34</v>
       </c>
       <c r="K606" s="24" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="L606" s="19"/>
       <c r="M606" s="19"/>
@@ -29056,7 +29056,7 @@
         <v>34</v>
       </c>
       <c r="K607" s="24" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="L607" s="19"/>
       <c r="M607" s="19"/>
@@ -29094,7 +29094,7 @@
         <v>34</v>
       </c>
       <c r="K608" s="24" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="L608" s="19"/>
       <c r="M608" s="19"/>
@@ -29106,7 +29106,7 @@
       <c r="S608" s="19"/>
       <c r="T608" s="25"/>
       <c r="U608" s="25" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="V608" s="1"/>
       <c r="W608" s="1"/>
@@ -29118,7 +29118,7 @@
       <c r="A609" s="19"/>
       <c r="B609" s="19"/>
       <c r="C609" s="19" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D609" s="19"/>
       <c r="E609" s="22"/>
@@ -29136,7 +29136,7 @@
         <v>39</v>
       </c>
       <c r="K609" s="24" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="L609" s="19"/>
       <c r="M609" s="19"/>
@@ -29174,7 +29174,7 @@
         <v>41</v>
       </c>
       <c r="K610" s="24" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="L610" s="19"/>
       <c r="M610" s="19"/>
@@ -29185,7 +29185,7 @@
       <c r="R610" s="19"/>
       <c r="S610" s="19"/>
       <c r="T610" s="9" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="U610" s="9"/>
       <c r="V610" s="1"/>
@@ -29198,7 +29198,7 @@
       <c r="A611" s="19"/>
       <c r="B611" s="19"/>
       <c r="C611" s="19" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D611" s="19"/>
       <c r="E611" s="22"/>
@@ -29216,7 +29216,7 @@
         <v>34</v>
       </c>
       <c r="K611" s="24" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="L611" s="19"/>
       <c r="M611" s="19"/>
@@ -29254,7 +29254,7 @@
         <v>34</v>
       </c>
       <c r="K612" s="24" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="L612" s="19"/>
       <c r="M612" s="19"/>
@@ -29266,7 +29266,7 @@
       <c r="S612" s="19"/>
       <c r="T612" s="25"/>
       <c r="U612" s="25" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="V612" s="1"/>
       <c r="W612" s="1"/>
@@ -29278,7 +29278,7 @@
       <c r="A613" s="19"/>
       <c r="B613" s="19"/>
       <c r="C613" s="19" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D613" s="19"/>
       <c r="E613" s="22"/>
@@ -29296,7 +29296,7 @@
         <v>39</v>
       </c>
       <c r="K613" s="24" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="L613" s="19"/>
       <c r="M613" s="19"/>
@@ -29334,7 +29334,7 @@
         <v>34</v>
       </c>
       <c r="K614" s="24" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="L614" s="19"/>
       <c r="M614" s="19"/>
@@ -29346,7 +29346,7 @@
       <c r="S614" s="19"/>
       <c r="T614" s="25"/>
       <c r="U614" s="25" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="V614" s="1"/>
       <c r="W614" s="1"/>
@@ -29358,7 +29358,7 @@
       <c r="A615" s="19"/>
       <c r="B615" s="19"/>
       <c r="C615" s="19" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="D615" s="19"/>
       <c r="E615" s="22"/>
@@ -29376,7 +29376,7 @@
         <v>174</v>
       </c>
       <c r="K615" s="24" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="L615" s="19"/>
       <c r="M615" s="19"/>
@@ -29426,7 +29426,7 @@
       <c r="S616" s="19"/>
       <c r="T616" s="25"/>
       <c r="U616" s="25" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="V616" s="1"/>
       <c r="W616" s="1"/>
@@ -29438,7 +29438,7 @@
       <c r="A617" s="19"/>
       <c r="B617" s="19"/>
       <c r="C617" s="19" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="D617" s="19"/>
       <c r="E617" s="22"/>
@@ -29456,7 +29456,7 @@
         <v>39</v>
       </c>
       <c r="K617" s="24" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="L617" s="19"/>
       <c r="M617" s="19"/>
@@ -29494,7 +29494,7 @@
         <v>34</v>
       </c>
       <c r="K618" s="24" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="L618" s="19"/>
       <c r="M618" s="19"/>
@@ -29506,7 +29506,7 @@
       <c r="S618" s="19"/>
       <c r="T618" s="25"/>
       <c r="U618" s="25" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="V618" s="1"/>
       <c r="W618" s="1"/>
@@ -29518,7 +29518,7 @@
       <c r="A619" s="19"/>
       <c r="B619" s="19"/>
       <c r="C619" s="19" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="D619" s="19" t="s">
         <v>185</v>
@@ -29527,7 +29527,7 @@
         <v>186</v>
       </c>
       <c r="F619" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G619" s="19" t="s">
         <v>376</v>
@@ -29536,7 +29536,7 @@
       <c r="I619" s="23"/>
       <c r="J619" s="23"/>
       <c r="K619" s="24" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="L619" s="19"/>
       <c r="M619" s="19"/>
@@ -29548,7 +29548,7 @@
       <c r="S619" s="19"/>
       <c r="T619" s="25"/>
       <c r="U619" s="25" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="V619" s="1"/>
       <c r="W619" s="1"/>
@@ -29560,14 +29560,14 @@
       <c r="A620" s="19"/>
       <c r="B620" s="19"/>
       <c r="C620" s="19" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D620" s="19" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="E620" s="22"/>
       <c r="F620" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G620" s="19" t="s">
         <v>376</v>
@@ -29580,7 +29580,7 @@
         <v>39</v>
       </c>
       <c r="K620" s="24" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="L620" s="19" t="s">
         <v>60</v>
@@ -29588,7 +29588,7 @@
       <c r="M620" s="19"/>
       <c r="N620" s="25"/>
       <c r="O620" s="25" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="P620" s="19"/>
       <c r="Q620" s="19"/>
@@ -29609,7 +29609,7 @@
       <c r="D621" s="19"/>
       <c r="E621" s="22"/>
       <c r="F621" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G621" s="19" t="s">
         <v>376</v>
@@ -29622,7 +29622,7 @@
         <v>34</v>
       </c>
       <c r="K621" s="24" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="L621" s="19"/>
       <c r="M621" s="19"/>
@@ -29647,7 +29647,7 @@
       <c r="D622" s="19"/>
       <c r="E622" s="22"/>
       <c r="F622" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G622" s="19" t="s">
         <v>376</v>
@@ -29660,7 +29660,7 @@
         <v>39</v>
       </c>
       <c r="K622" s="24" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="L622" s="19"/>
       <c r="M622" s="19"/>
@@ -29685,7 +29685,7 @@
       <c r="D623" s="19"/>
       <c r="E623" s="22"/>
       <c r="F623" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G623" s="19" t="s">
         <v>376</v>
@@ -29698,7 +29698,7 @@
         <v>34</v>
       </c>
       <c r="K623" s="24" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="L623" s="19"/>
       <c r="M623" s="19"/>
@@ -29723,7 +29723,7 @@
       <c r="D624" s="19"/>
       <c r="E624" s="22"/>
       <c r="F624" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G624" s="19" t="s">
         <v>376</v>
@@ -29736,7 +29736,7 @@
         <v>39</v>
       </c>
       <c r="K624" s="24" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="L624" s="19"/>
       <c r="M624" s="19"/>
@@ -29761,7 +29761,7 @@
       <c r="D625" s="19"/>
       <c r="E625" s="22"/>
       <c r="F625" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G625" s="19" t="s">
         <v>376</v>
@@ -29774,7 +29774,7 @@
         <v>54</v>
       </c>
       <c r="K625" s="24" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="L625" s="19"/>
       <c r="M625" s="19"/>
@@ -29799,7 +29799,7 @@
       <c r="D626" s="19"/>
       <c r="E626" s="22"/>
       <c r="F626" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G626" s="19" t="s">
         <v>376</v>
@@ -29812,7 +29812,7 @@
         <v>39</v>
       </c>
       <c r="K626" s="24" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="L626" s="19"/>
       <c r="M626" s="19"/>
@@ -29837,7 +29837,7 @@
       <c r="D627" s="19"/>
       <c r="E627" s="22"/>
       <c r="F627" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G627" s="19" t="s">
         <v>376</v>
@@ -29850,7 +29850,7 @@
         <v>39</v>
       </c>
       <c r="K627" s="24" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="L627" s="19"/>
       <c r="M627" s="19"/>
@@ -29875,7 +29875,7 @@
       <c r="D628" s="19"/>
       <c r="E628" s="22"/>
       <c r="F628" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G628" s="19" t="s">
         <v>376</v>
@@ -29888,7 +29888,7 @@
         <v>39</v>
       </c>
       <c r="K628" s="24" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="L628" s="19"/>
       <c r="M628" s="19"/>
@@ -29913,7 +29913,7 @@
       <c r="D629" s="19"/>
       <c r="E629" s="22"/>
       <c r="F629" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G629" s="19" t="s">
         <v>376</v>
@@ -29926,7 +29926,7 @@
         <v>41</v>
       </c>
       <c r="K629" s="24" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="L629" s="19"/>
       <c r="M629" s="19"/>
@@ -29938,7 +29938,7 @@
       <c r="S629" s="14"/>
       <c r="T629" s="9"/>
       <c r="U629" s="9" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="V629" s="1"/>
       <c r="W629" s="1"/>
@@ -29950,12 +29950,12 @@
       <c r="A630" s="19"/>
       <c r="B630" s="19"/>
       <c r="C630" s="19" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="D630" s="19"/>
       <c r="E630" s="22"/>
       <c r="F630" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G630" s="19" t="s">
         <v>383</v>
@@ -29968,7 +29968,7 @@
         <v>34</v>
       </c>
       <c r="K630" s="24" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="L630" s="19" t="s">
         <v>60</v>
@@ -29976,7 +29976,7 @@
       <c r="M630" s="19"/>
       <c r="N630" s="25"/>
       <c r="O630" s="25" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="P630" s="19"/>
       <c r="Q630" s="19"/>
@@ -29997,7 +29997,7 @@
       <c r="D631" s="19"/>
       <c r="E631" s="22"/>
       <c r="F631" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G631" s="19" t="s">
         <v>383</v>
@@ -30010,7 +30010,7 @@
         <v>34</v>
       </c>
       <c r="K631" s="24" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="L631" s="19"/>
       <c r="M631" s="19"/>
@@ -30035,7 +30035,7 @@
       <c r="D632" s="19"/>
       <c r="E632" s="22"/>
       <c r="F632" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G632" s="19" t="s">
         <v>383</v>
@@ -30048,7 +30048,7 @@
         <v>39</v>
       </c>
       <c r="K632" s="24" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="L632" s="19"/>
       <c r="M632" s="19"/>
@@ -30073,7 +30073,7 @@
       <c r="D633" s="19"/>
       <c r="E633" s="22"/>
       <c r="F633" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G633" s="19" t="s">
         <v>383</v>
@@ -30086,7 +30086,7 @@
         <v>41</v>
       </c>
       <c r="K633" s="24" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="L633" s="19"/>
       <c r="M633" s="19"/>
@@ -30111,7 +30111,7 @@
       <c r="D634" s="19"/>
       <c r="E634" s="22"/>
       <c r="F634" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G634" s="19" t="s">
         <v>383</v>
@@ -30124,7 +30124,7 @@
         <v>39</v>
       </c>
       <c r="K634" s="24" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="L634" s="19"/>
       <c r="M634" s="19"/>
@@ -30149,7 +30149,7 @@
       <c r="D635" s="19"/>
       <c r="E635" s="22"/>
       <c r="F635" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G635" s="19" t="s">
         <v>383</v>
@@ -30162,7 +30162,7 @@
         <v>221</v>
       </c>
       <c r="K635" s="24" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="L635" s="19"/>
       <c r="M635" s="19"/>
@@ -30187,7 +30187,7 @@
       <c r="D636" s="19"/>
       <c r="E636" s="22"/>
       <c r="F636" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G636" s="19" t="s">
         <v>383</v>
@@ -30200,7 +30200,7 @@
         <v>34</v>
       </c>
       <c r="K636" s="24" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="L636" s="19"/>
       <c r="M636" s="19"/>
@@ -30225,7 +30225,7 @@
       <c r="D637" s="19"/>
       <c r="E637" s="22"/>
       <c r="F637" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G637" s="19" t="s">
         <v>383</v>
@@ -30238,7 +30238,7 @@
         <v>174</v>
       </c>
       <c r="K637" s="24" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="L637" s="19"/>
       <c r="M637" s="19"/>
@@ -30263,7 +30263,7 @@
       <c r="D638" s="19"/>
       <c r="E638" s="22"/>
       <c r="F638" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G638" s="19" t="s">
         <v>383</v>
@@ -30276,7 +30276,7 @@
         <v>34</v>
       </c>
       <c r="K638" s="24" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="L638" s="19"/>
       <c r="M638" s="19"/>
@@ -30288,7 +30288,7 @@
       <c r="S638" s="14"/>
       <c r="T638" s="9"/>
       <c r="U638" s="9" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="V638" s="1"/>
       <c r="W638" s="1"/>
@@ -30300,12 +30300,12 @@
       <c r="A639" s="19"/>
       <c r="B639" s="19"/>
       <c r="C639" s="19" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="D639" s="19"/>
       <c r="E639" s="22"/>
       <c r="F639" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G639" s="19" t="s">
         <v>332</v>
@@ -30318,7 +30318,7 @@
         <v>54</v>
       </c>
       <c r="K639" s="24" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="L639" s="19"/>
       <c r="M639" s="19"/>
@@ -30345,7 +30345,7 @@
       <c r="D640" s="19"/>
       <c r="E640" s="22"/>
       <c r="F640" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G640" s="19" t="s">
         <v>332</v>
@@ -30358,7 +30358,7 @@
         <v>39</v>
       </c>
       <c r="K640" s="24" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="L640" s="19"/>
       <c r="M640" s="19"/>
@@ -30383,13 +30383,13 @@
       <c r="D641" s="19"/>
       <c r="E641" s="22"/>
       <c r="F641" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G641" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H641" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I641" s="19" t="s">
         <v>196</v>
@@ -30398,7 +30398,7 @@
         <v>39</v>
       </c>
       <c r="K641" s="24" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="L641" s="19"/>
       <c r="M641" s="19"/>
@@ -30423,7 +30423,7 @@
       <c r="D642" s="19"/>
       <c r="E642" s="22"/>
       <c r="F642" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G642" s="19" t="s">
         <v>332</v>
@@ -30436,7 +30436,7 @@
         <v>54</v>
       </c>
       <c r="K642" s="24" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="L642" s="19"/>
       <c r="M642" s="19"/>
@@ -30461,7 +30461,7 @@
       <c r="D643" s="19"/>
       <c r="E643" s="22"/>
       <c r="F643" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G643" s="19" t="s">
         <v>332</v>
@@ -30474,7 +30474,7 @@
         <v>41</v>
       </c>
       <c r="K643" s="55" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="L643" s="19"/>
       <c r="M643" s="19"/>
@@ -30499,7 +30499,7 @@
       <c r="D644" s="19"/>
       <c r="E644" s="22"/>
       <c r="F644" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G644" s="19" t="s">
         <v>332</v>
@@ -30512,7 +30512,7 @@
         <v>39</v>
       </c>
       <c r="K644" s="24" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="L644" s="19"/>
       <c r="M644" s="19"/>
@@ -30537,13 +30537,13 @@
       <c r="D645" s="19"/>
       <c r="E645" s="22"/>
       <c r="F645" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G645" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H645" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I645" s="19" t="s">
         <v>196</v>
@@ -30552,7 +30552,7 @@
         <v>221</v>
       </c>
       <c r="K645" s="24" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="L645" s="19"/>
       <c r="M645" s="19"/>
@@ -30577,13 +30577,13 @@
       <c r="D646" s="19"/>
       <c r="E646" s="22"/>
       <c r="F646" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G646" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H646" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I646" s="19" t="s">
         <v>196</v>
@@ -30592,7 +30592,7 @@
         <v>221</v>
       </c>
       <c r="K646" s="24" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="L646" s="19"/>
       <c r="M646" s="19"/>
@@ -30617,7 +30617,7 @@
       <c r="D647" s="19"/>
       <c r="E647" s="22"/>
       <c r="F647" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G647" s="19" t="s">
         <v>332</v>
@@ -30630,7 +30630,7 @@
         <v>221</v>
       </c>
       <c r="K647" s="24" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="L647" s="19"/>
       <c r="M647" s="19"/>
@@ -30655,13 +30655,13 @@
       <c r="D648" s="19"/>
       <c r="E648" s="22"/>
       <c r="F648" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G648" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H648" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I648" s="19" t="s">
         <v>196</v>
@@ -30670,7 +30670,7 @@
         <v>221</v>
       </c>
       <c r="K648" s="24" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="L648" s="19"/>
       <c r="M648" s="19"/>
@@ -30695,13 +30695,13 @@
       <c r="D649" s="19"/>
       <c r="E649" s="22"/>
       <c r="F649" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G649" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H649" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I649" s="19" t="s">
         <v>196</v>
@@ -30710,7 +30710,7 @@
         <v>221</v>
       </c>
       <c r="K649" s="24" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="L649" s="19"/>
       <c r="M649" s="19"/>
@@ -30735,13 +30735,13 @@
       <c r="D650" s="19"/>
       <c r="E650" s="22"/>
       <c r="F650" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G650" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H650" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I650" s="19" t="s">
         <v>196</v>
@@ -30750,7 +30750,7 @@
         <v>221</v>
       </c>
       <c r="K650" s="24" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="L650" s="19"/>
       <c r="M650" s="19"/>
@@ -30775,13 +30775,13 @@
       <c r="D651" s="19"/>
       <c r="E651" s="22"/>
       <c r="F651" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G651" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H651" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I651" s="19" t="s">
         <v>196</v>
@@ -30790,7 +30790,7 @@
         <v>221</v>
       </c>
       <c r="K651" s="24" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="L651" s="19"/>
       <c r="M651" s="19"/>
@@ -30815,7 +30815,7 @@
       <c r="D652" s="19"/>
       <c r="E652" s="22"/>
       <c r="F652" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G652" s="19" t="s">
         <v>332</v>
@@ -30828,7 +30828,7 @@
         <v>221</v>
       </c>
       <c r="K652" s="24" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="L652" s="19"/>
       <c r="M652" s="19"/>
@@ -30853,13 +30853,13 @@
       <c r="D653" s="19"/>
       <c r="E653" s="22"/>
       <c r="F653" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G653" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H653" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I653" s="19" t="s">
         <v>196</v>
@@ -30868,7 +30868,7 @@
         <v>221</v>
       </c>
       <c r="K653" s="24" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="L653" s="19"/>
       <c r="M653" s="19"/>
@@ -30893,7 +30893,7 @@
       <c r="D654" s="19"/>
       <c r="E654" s="22"/>
       <c r="F654" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G654" s="19" t="s">
         <v>332</v>
@@ -30906,7 +30906,7 @@
         <v>34</v>
       </c>
       <c r="K654" s="24" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="L654" s="19"/>
       <c r="M654" s="19"/>
@@ -30931,7 +30931,7 @@
       <c r="D655" s="19"/>
       <c r="E655" s="22"/>
       <c r="F655" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G655" s="19" t="s">
         <v>332</v>
@@ -30944,14 +30944,14 @@
         <v>34</v>
       </c>
       <c r="K655" s="24" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="L655" s="19" t="s">
         <v>149</v>
       </c>
       <c r="M655" s="19"/>
       <c r="N655" s="25" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="O655" s="25"/>
       <c r="P655" s="19"/>
@@ -30973,13 +30973,13 @@
       <c r="D656" s="19"/>
       <c r="E656" s="22"/>
       <c r="F656" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G656" s="19" t="s">
         <v>332</v>
       </c>
       <c r="H656" s="23" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="I656" s="19" t="s">
         <v>196</v>
@@ -30988,7 +30988,7 @@
         <v>703</v>
       </c>
       <c r="K656" s="24" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="L656" s="19"/>
       <c r="M656" s="19"/>
@@ -30998,7 +30998,7 @@
       <c r="Q656" s="19"/>
       <c r="R656" s="14"/>
       <c r="S656" s="14" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="T656" s="9"/>
       <c r="U656" s="9"/>
@@ -31015,7 +31015,7 @@
       <c r="D657" s="19"/>
       <c r="E657" s="22"/>
       <c r="F657" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G657" s="19" t="s">
         <v>332</v>
@@ -31028,7 +31028,7 @@
         <v>39</v>
       </c>
       <c r="K657" s="24" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="L657" s="19"/>
       <c r="M657" s="19"/>
@@ -31053,7 +31053,7 @@
       <c r="D658" s="19"/>
       <c r="E658" s="22"/>
       <c r="F658" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G658" s="19" t="s">
         <v>332</v>
@@ -31066,7 +31066,7 @@
         <v>54</v>
       </c>
       <c r="K658" s="24" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="L658" s="19"/>
       <c r="M658" s="19"/>
@@ -31091,7 +31091,7 @@
       <c r="D659" s="19"/>
       <c r="E659" s="22"/>
       <c r="F659" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G659" s="19" t="s">
         <v>332</v>
@@ -31104,7 +31104,7 @@
         <v>54</v>
       </c>
       <c r="K659" s="24" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="L659" s="19" t="s">
         <v>60</v>
@@ -31112,7 +31112,7 @@
       <c r="M659" s="19"/>
       <c r="N659" s="25"/>
       <c r="O659" s="25" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="P659" s="19"/>
       <c r="Q659" s="19"/>
@@ -31120,7 +31120,7 @@
       <c r="S659" s="14"/>
       <c r="T659" s="9"/>
       <c r="U659" s="9" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="V659" s="1"/>
       <c r="W659" s="1"/>
@@ -31132,12 +31132,12 @@
       <c r="A660" s="19"/>
       <c r="B660" s="19"/>
       <c r="C660" s="19" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D660" s="19"/>
       <c r="E660" s="22"/>
       <c r="F660" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G660" s="19" t="s">
         <v>332</v>
@@ -31152,7 +31152,7 @@
         <v>34</v>
       </c>
       <c r="K660" s="24" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="L660" s="19"/>
       <c r="M660" s="19"/>
@@ -31179,7 +31179,7 @@
       <c r="D661" s="19"/>
       <c r="E661" s="22"/>
       <c r="F661" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G661" s="19" t="s">
         <v>332</v>
@@ -31194,7 +31194,7 @@
         <v>39</v>
       </c>
       <c r="K661" s="24" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="L661" s="19"/>
       <c r="M661" s="19"/>
@@ -31219,7 +31219,7 @@
       <c r="D662" s="19"/>
       <c r="E662" s="22"/>
       <c r="F662" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G662" s="19" t="s">
         <v>332</v>
@@ -31234,7 +31234,7 @@
         <v>34</v>
       </c>
       <c r="K662" s="24" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="L662" s="19"/>
       <c r="M662" s="19"/>
@@ -31259,7 +31259,7 @@
       <c r="D663" s="19"/>
       <c r="E663" s="22"/>
       <c r="F663" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G663" s="19" t="s">
         <v>332</v>
@@ -31274,7 +31274,7 @@
         <v>54</v>
       </c>
       <c r="K663" s="24" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="L663" s="19"/>
       <c r="M663" s="19"/>
@@ -31299,7 +31299,7 @@
       <c r="D664" s="19"/>
       <c r="E664" s="22"/>
       <c r="F664" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G664" s="19" t="s">
         <v>332</v>
@@ -31314,7 +31314,7 @@
         <v>39</v>
       </c>
       <c r="K664" s="24" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="L664" s="19"/>
       <c r="M664" s="19"/>
@@ -31339,7 +31339,7 @@
       <c r="D665" s="19"/>
       <c r="E665" s="22"/>
       <c r="F665" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G665" s="19" t="s">
         <v>332</v>
@@ -31354,7 +31354,7 @@
         <v>34</v>
       </c>
       <c r="K665" s="24" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="L665" s="19"/>
       <c r="M665" s="19"/>
@@ -31379,7 +31379,7 @@
       <c r="D666" s="19"/>
       <c r="E666" s="22"/>
       <c r="F666" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G666" s="19" t="s">
         <v>332</v>
@@ -31392,7 +31392,7 @@
         <v>54</v>
       </c>
       <c r="K666" s="24" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="L666" s="19"/>
       <c r="M666" s="19"/>
@@ -31417,7 +31417,7 @@
       <c r="D667" s="19"/>
       <c r="E667" s="22"/>
       <c r="F667" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G667" s="19" t="s">
         <v>332</v>
@@ -31432,7 +31432,7 @@
         <v>747</v>
       </c>
       <c r="K667" s="24" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="L667" s="19"/>
       <c r="M667" s="19"/>
@@ -31457,7 +31457,7 @@
       <c r="D668" s="19"/>
       <c r="E668" s="22"/>
       <c r="F668" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G668" s="19" t="s">
         <v>332</v>
@@ -31472,7 +31472,7 @@
         <v>39</v>
       </c>
       <c r="K668" s="24" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="L668" s="19" t="s">
         <v>60</v>
@@ -31480,7 +31480,7 @@
       <c r="M668" s="19"/>
       <c r="N668" s="25"/>
       <c r="O668" s="25" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="P668" s="19"/>
       <c r="Q668" s="19"/>
@@ -31501,7 +31501,7 @@
       <c r="D669" s="19"/>
       <c r="E669" s="22"/>
       <c r="F669" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G669" s="19" t="s">
         <v>332</v>
@@ -31516,7 +31516,7 @@
         <v>39</v>
       </c>
       <c r="K669" s="24" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="L669" s="19"/>
       <c r="M669" s="19"/>
@@ -31541,7 +31541,7 @@
       <c r="D670" s="19"/>
       <c r="E670" s="22"/>
       <c r="F670" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G670" s="19" t="s">
         <v>332</v>
@@ -31556,7 +31556,7 @@
         <v>34</v>
       </c>
       <c r="K670" s="24" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="L670" s="19" t="s">
         <v>60</v>
@@ -31564,7 +31564,7 @@
       <c r="M670" s="19"/>
       <c r="N670" s="25"/>
       <c r="O670" s="25" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="P670" s="19"/>
       <c r="Q670" s="19"/>
@@ -31585,7 +31585,7 @@
       <c r="D671" s="19"/>
       <c r="E671" s="22"/>
       <c r="F671" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G671" s="19" t="s">
         <v>332</v>
@@ -31598,7 +31598,7 @@
         <v>39</v>
       </c>
       <c r="K671" s="24" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="L671" s="19"/>
       <c r="M671" s="19"/>
@@ -31623,7 +31623,7 @@
       <c r="D672" s="19"/>
       <c r="E672" s="22"/>
       <c r="F672" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G672" s="19" t="s">
         <v>332</v>
@@ -31636,7 +31636,7 @@
         <v>221</v>
       </c>
       <c r="K672" s="24" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="L672" s="19"/>
       <c r="M672" s="19"/>
@@ -31661,7 +31661,7 @@
       <c r="D673" s="19"/>
       <c r="E673" s="22"/>
       <c r="F673" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G673" s="19" t="s">
         <v>332</v>
@@ -31674,7 +31674,7 @@
         <v>221</v>
       </c>
       <c r="K673" s="24" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="L673" s="19"/>
       <c r="M673" s="19"/>
@@ -31699,7 +31699,7 @@
       <c r="D674" s="19"/>
       <c r="E674" s="22"/>
       <c r="F674" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G674" s="19" t="s">
         <v>332</v>
@@ -31712,7 +31712,7 @@
         <v>221</v>
       </c>
       <c r="K674" s="24" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="L674" s="19"/>
       <c r="M674" s="19"/>
@@ -31737,7 +31737,7 @@
       <c r="D675" s="19"/>
       <c r="E675" s="22"/>
       <c r="F675" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G675" s="19" t="s">
         <v>332</v>
@@ -31750,21 +31750,21 @@
         <v>174</v>
       </c>
       <c r="K675" s="24" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="L675" s="19" t="s">
         <v>149</v>
       </c>
       <c r="M675" s="19"/>
       <c r="N675" s="25" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="O675" s="25"/>
       <c r="P675" s="19"/>
       <c r="Q675" s="19"/>
       <c r="R675" s="14"/>
       <c r="S675" s="14" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="T675" s="9"/>
       <c r="U675" s="9"/>
@@ -31781,7 +31781,7 @@
       <c r="D676" s="19"/>
       <c r="E676" s="22"/>
       <c r="F676" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G676" s="19" t="s">
         <v>332</v>
@@ -31796,7 +31796,7 @@
         <v>747</v>
       </c>
       <c r="K676" s="24" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="L676" s="19"/>
       <c r="M676" s="19"/>
@@ -31821,7 +31821,7 @@
       <c r="D677" s="19"/>
       <c r="E677" s="22"/>
       <c r="F677" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G677" s="19" t="s">
         <v>332</v>
@@ -31836,7 +31836,7 @@
         <v>747</v>
       </c>
       <c r="K677" s="24" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="L677" s="19"/>
       <c r="M677" s="19"/>
@@ -31861,7 +31861,7 @@
       <c r="D678" s="19"/>
       <c r="E678" s="22"/>
       <c r="F678" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G678" s="19" t="s">
         <v>332</v>
@@ -31876,7 +31876,7 @@
         <v>39</v>
       </c>
       <c r="K678" s="24" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="L678" s="19"/>
       <c r="M678" s="19"/>
@@ -31901,7 +31901,7 @@
       <c r="D679" s="19"/>
       <c r="E679" s="22"/>
       <c r="F679" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G679" s="19" t="s">
         <v>332</v>
@@ -31916,7 +31916,7 @@
         <v>34</v>
       </c>
       <c r="K679" s="24" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="L679" s="19"/>
       <c r="M679" s="19"/>
@@ -31941,7 +31941,7 @@
       <c r="D680" s="19"/>
       <c r="E680" s="22"/>
       <c r="F680" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G680" s="19" t="s">
         <v>332</v>
@@ -31956,7 +31956,7 @@
         <v>34</v>
       </c>
       <c r="K680" s="24" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="L680" s="19"/>
       <c r="M680" s="19"/>
@@ -31981,7 +31981,7 @@
       <c r="D681" s="19"/>
       <c r="E681" s="22"/>
       <c r="F681" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G681" s="19" t="s">
         <v>332</v>
@@ -31996,7 +31996,7 @@
         <v>708</v>
       </c>
       <c r="K681" s="24" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="L681" s="19"/>
       <c r="M681" s="19"/>
@@ -32010,7 +32010,7 @@
       </c>
       <c r="T681" s="9"/>
       <c r="U681" s="9" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="V681" s="1"/>
       <c r="W681" s="1"/>
@@ -32022,15 +32022,15 @@
       <c r="A682" s="19"/>
       <c r="B682" s="19"/>
       <c r="C682" s="19" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D682" s="19"/>
       <c r="E682" s="22"/>
       <c r="F682" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G682" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H682" s="23" t="s">
         <v>220</v>
@@ -32040,7 +32040,7 @@
         <v>54</v>
       </c>
       <c r="K682" s="24" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="L682" s="19"/>
       <c r="M682" s="19"/>
@@ -32065,13 +32065,13 @@
       <c r="D683" s="19"/>
       <c r="E683" s="22"/>
       <c r="F683" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G683" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H683" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H683" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I683" s="19" t="s">
         <v>196</v>
@@ -32080,7 +32080,7 @@
         <v>174</v>
       </c>
       <c r="K683" s="24" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="L683" s="19"/>
       <c r="M683" s="19"/>
@@ -32105,10 +32105,10 @@
       <c r="D684" s="19"/>
       <c r="E684" s="22"/>
       <c r="F684" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G684" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H684" s="23" t="s">
         <v>220</v>
@@ -32118,7 +32118,7 @@
         <v>54</v>
       </c>
       <c r="K684" s="24" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="L684" s="19"/>
       <c r="M684" s="19"/>
@@ -32143,13 +32143,13 @@
       <c r="D685" s="19"/>
       <c r="E685" s="22"/>
       <c r="F685" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G685" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H685" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H685" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I685" s="19" t="s">
         <v>196</v>
@@ -32158,7 +32158,7 @@
         <v>174</v>
       </c>
       <c r="K685" s="24" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="L685" s="19"/>
       <c r="M685" s="19"/>
@@ -32183,13 +32183,13 @@
       <c r="D686" s="19"/>
       <c r="E686" s="22"/>
       <c r="F686" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G686" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H686" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H686" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I686" s="19" t="s">
         <v>196</v>
@@ -32198,7 +32198,7 @@
         <v>54</v>
       </c>
       <c r="K686" s="24" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="L686" s="19"/>
       <c r="M686" s="19"/>
@@ -32223,10 +32223,10 @@
       <c r="D687" s="19"/>
       <c r="E687" s="22"/>
       <c r="F687" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G687" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H687" s="23" t="s">
         <v>236</v>
@@ -32236,7 +32236,7 @@
         <v>39</v>
       </c>
       <c r="K687" s="24" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="L687" s="19"/>
       <c r="M687" s="19"/>
@@ -32261,13 +32261,13 @@
       <c r="D688" s="19"/>
       <c r="E688" s="22"/>
       <c r="F688" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G688" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H688" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H688" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I688" s="19" t="s">
         <v>196</v>
@@ -32276,7 +32276,7 @@
         <v>39</v>
       </c>
       <c r="K688" s="24" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="L688" s="19"/>
       <c r="M688" s="19"/>
@@ -32301,13 +32301,13 @@
       <c r="D689" s="19"/>
       <c r="E689" s="22"/>
       <c r="F689" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G689" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H689" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H689" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I689" s="19" t="s">
         <v>196</v>
@@ -32316,7 +32316,7 @@
         <v>39</v>
       </c>
       <c r="K689" s="24" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="L689" s="19"/>
       <c r="M689" s="19"/>
@@ -32341,13 +32341,13 @@
       <c r="D690" s="19"/>
       <c r="E690" s="22"/>
       <c r="F690" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G690" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H690" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H690" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I690" s="19" t="s">
         <v>196</v>
@@ -32356,7 +32356,7 @@
         <v>174</v>
       </c>
       <c r="K690" s="24" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="L690" s="19"/>
       <c r="M690" s="19"/>
@@ -32381,13 +32381,13 @@
       <c r="D691" s="19"/>
       <c r="E691" s="22"/>
       <c r="F691" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G691" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H691" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H691" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I691" s="19" t="s">
         <v>196</v>
@@ -32396,7 +32396,7 @@
         <v>54</v>
       </c>
       <c r="K691" s="24" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="L691" s="19"/>
       <c r="M691" s="19"/>
@@ -32421,13 +32421,13 @@
       <c r="D692" s="19"/>
       <c r="E692" s="22"/>
       <c r="F692" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G692" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H692" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H692" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I692" s="19" t="s">
         <v>196</v>
@@ -32436,7 +32436,7 @@
         <v>174</v>
       </c>
       <c r="K692" s="24" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="L692" s="19"/>
       <c r="M692" s="19"/>
@@ -32461,13 +32461,13 @@
       <c r="D693" s="19"/>
       <c r="E693" s="22"/>
       <c r="F693" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G693" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H693" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H693" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I693" s="19" t="s">
         <v>196</v>
@@ -32476,7 +32476,7 @@
         <v>174</v>
       </c>
       <c r="K693" s="24" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="L693" s="19"/>
       <c r="M693" s="19"/>
@@ -32501,13 +32501,13 @@
       <c r="D694" s="19"/>
       <c r="E694" s="22"/>
       <c r="F694" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G694" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H694" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H694" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I694" s="19" t="s">
         <v>196</v>
@@ -32516,7 +32516,7 @@
         <v>174</v>
       </c>
       <c r="K694" s="24" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="L694" s="19"/>
       <c r="M694" s="19"/>
@@ -32541,13 +32541,13 @@
       <c r="D695" s="19"/>
       <c r="E695" s="22"/>
       <c r="F695" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G695" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H695" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H695" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I695" s="19" t="s">
         <v>196</v>
@@ -32556,7 +32556,7 @@
         <v>174</v>
       </c>
       <c r="K695" s="24" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="L695" s="19"/>
       <c r="M695" s="19"/>
@@ -32581,13 +32581,13 @@
       <c r="D696" s="19"/>
       <c r="E696" s="22"/>
       <c r="F696" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G696" s="19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H696" s="23" t="s">
         <v>1138</v>
-      </c>
-      <c r="H696" s="23" t="s">
-        <v>1140</v>
       </c>
       <c r="I696" s="19" t="s">
         <v>196</v>
@@ -32596,7 +32596,7 @@
         <v>41</v>
       </c>
       <c r="K696" s="24" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="L696" s="19"/>
       <c r="M696" s="19"/>
@@ -32621,10 +32621,10 @@
       <c r="D697" s="19"/>
       <c r="E697" s="22"/>
       <c r="F697" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G697" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H697" s="23" t="s">
         <v>236</v>
@@ -32634,7 +32634,7 @@
         <v>39</v>
       </c>
       <c r="K697" s="24" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="L697" s="19"/>
       <c r="M697" s="19"/>
@@ -32659,10 +32659,10 @@
       <c r="D698" s="19"/>
       <c r="E698" s="22"/>
       <c r="F698" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G698" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H698" s="23" t="s">
         <v>220</v>
@@ -32672,7 +32672,7 @@
         <v>34</v>
       </c>
       <c r="K698" s="24" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="L698" s="19"/>
       <c r="M698" s="19"/>
@@ -32699,10 +32699,10 @@
       <c r="D699" s="19"/>
       <c r="E699" s="22"/>
       <c r="F699" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G699" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H699" s="23" t="s">
         <v>236</v>
@@ -32720,7 +32720,7 @@
       <c r="M699" s="19"/>
       <c r="N699" s="25"/>
       <c r="O699" s="25" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="P699" s="19"/>
       <c r="Q699" s="19"/>
@@ -32741,10 +32741,10 @@
       <c r="D700" s="19"/>
       <c r="E700" s="22"/>
       <c r="F700" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G700" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H700" s="23" t="s">
         <v>236</v>
@@ -32754,14 +32754,14 @@
         <v>39</v>
       </c>
       <c r="K700" s="24" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="L700" s="19" t="s">
         <v>149</v>
       </c>
       <c r="M700" s="19"/>
       <c r="N700" s="25" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="O700" s="25"/>
       <c r="P700" s="19"/>
@@ -32783,10 +32783,10 @@
       <c r="D701" s="19"/>
       <c r="E701" s="22"/>
       <c r="F701" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G701" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H701" s="23" t="s">
         <v>236</v>
@@ -32796,7 +32796,7 @@
         <v>174</v>
       </c>
       <c r="K701" s="24" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="L701" s="19"/>
       <c r="M701" s="19"/>
@@ -32821,10 +32821,10 @@
       <c r="D702" s="19"/>
       <c r="E702" s="22"/>
       <c r="F702" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G702" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H702" s="23" t="s">
         <v>236</v>
@@ -32834,7 +32834,7 @@
         <v>54</v>
       </c>
       <c r="K702" s="24" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="L702" s="19"/>
       <c r="M702" s="19"/>
@@ -32859,10 +32859,10 @@
       <c r="D703" s="19"/>
       <c r="E703" s="22"/>
       <c r="F703" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G703" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H703" s="23" t="s">
         <v>236</v>
@@ -32872,7 +32872,7 @@
         <v>54</v>
       </c>
       <c r="K703" s="24" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="L703" s="19"/>
       <c r="M703" s="19"/>
@@ -32897,10 +32897,10 @@
       <c r="D704" s="19"/>
       <c r="E704" s="22"/>
       <c r="F704" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G704" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H704" s="23" t="s">
         <v>236</v>
@@ -32910,7 +32910,7 @@
         <v>174</v>
       </c>
       <c r="K704" s="24" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="L704" s="19"/>
       <c r="M704" s="19"/>
@@ -32935,10 +32935,10 @@
       <c r="D705" s="19"/>
       <c r="E705" s="22"/>
       <c r="F705" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G705" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H705" s="23" t="s">
         <v>236</v>
@@ -32948,7 +32948,7 @@
         <v>174</v>
       </c>
       <c r="K705" s="24" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="L705" s="19" t="s">
         <v>60</v>
@@ -32956,7 +32956,7 @@
       <c r="M705" s="19"/>
       <c r="N705" s="25"/>
       <c r="O705" s="25" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="P705" s="19"/>
       <c r="Q705" s="19"/>
@@ -32977,10 +32977,10 @@
       <c r="D706" s="19"/>
       <c r="E706" s="22"/>
       <c r="F706" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G706" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H706" s="23" t="s">
         <v>236</v>
@@ -32990,7 +32990,7 @@
         <v>41</v>
       </c>
       <c r="K706" s="24" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="L706" s="19"/>
       <c r="M706" s="19"/>
@@ -33015,10 +33015,10 @@
       <c r="D707" s="19"/>
       <c r="E707" s="22"/>
       <c r="F707" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G707" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H707" s="23" t="s">
         <v>236</v>
@@ -33028,7 +33028,7 @@
         <v>41</v>
       </c>
       <c r="K707" s="24" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="L707" s="19"/>
       <c r="M707" s="19"/>
@@ -33053,10 +33053,10 @@
       <c r="D708" s="19"/>
       <c r="E708" s="22"/>
       <c r="F708" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G708" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H708" s="23" t="s">
         <v>236</v>
@@ -33066,7 +33066,7 @@
         <v>221</v>
       </c>
       <c r="K708" s="24" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="L708" s="19"/>
       <c r="M708" s="19"/>
@@ -33091,10 +33091,10 @@
       <c r="D709" s="19"/>
       <c r="E709" s="22"/>
       <c r="F709" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G709" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H709" s="23" t="s">
         <v>220</v>
@@ -33104,7 +33104,7 @@
         <v>174</v>
       </c>
       <c r="K709" s="24" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="L709" s="19"/>
       <c r="M709" s="19"/>
@@ -33129,10 +33129,10 @@
       <c r="D710" s="19"/>
       <c r="E710" s="22"/>
       <c r="F710" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G710" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H710" s="23" t="s">
         <v>236</v>
@@ -33142,7 +33142,7 @@
         <v>174</v>
       </c>
       <c r="K710" s="24" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="L710" s="19"/>
       <c r="M710" s="19"/>
@@ -33167,10 +33167,10 @@
       <c r="D711" s="19"/>
       <c r="E711" s="22"/>
       <c r="F711" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G711" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H711" s="23" t="s">
         <v>236</v>
@@ -33180,7 +33180,7 @@
         <v>39</v>
       </c>
       <c r="K711" s="24" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="L711" s="19" t="s">
         <v>60</v>
@@ -33188,7 +33188,7 @@
       <c r="M711" s="19"/>
       <c r="N711" s="25"/>
       <c r="O711" s="25" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="P711" s="19"/>
       <c r="Q711" s="19"/>
@@ -33209,10 +33209,10 @@
       <c r="D712" s="19"/>
       <c r="E712" s="22"/>
       <c r="F712" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G712" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H712" s="23" t="s">
         <v>236</v>
@@ -33222,7 +33222,7 @@
         <v>39</v>
       </c>
       <c r="K712" s="24" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="L712" s="19"/>
       <c r="M712" s="19"/>
@@ -33247,10 +33247,10 @@
       <c r="D713" s="19"/>
       <c r="E713" s="22"/>
       <c r="F713" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G713" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H713" s="23" t="s">
         <v>236</v>
@@ -33260,7 +33260,7 @@
         <v>39</v>
       </c>
       <c r="K713" s="24" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="L713" s="19"/>
       <c r="M713" s="19"/>
@@ -33272,7 +33272,7 @@
       <c r="S713" s="14"/>
       <c r="T713" s="25"/>
       <c r="U713" s="25" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="V713" s="1"/>
       <c r="W713" s="1"/>
@@ -33284,7 +33284,7 @@
       <c r="A714" s="19"/>
       <c r="B714" s="19"/>
       <c r="C714" s="19" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="D714" s="19" t="s">
         <v>185</v>
@@ -33293,16 +33293,16 @@
         <v>186</v>
       </c>
       <c r="F714" s="22" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G714" s="19" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H714" s="23"/>
       <c r="I714" s="23"/>
       <c r="J714" s="23"/>
       <c r="K714" s="24" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="L714" s="19"/>
       <c r="M714" s="19"/>
@@ -33314,7 +33314,7 @@
       <c r="S714" s="19"/>
       <c r="T714" s="25"/>
       <c r="U714" s="25" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="V714" s="1"/>
       <c r="W714" s="1"/>
@@ -33326,10 +33326,10 @@
       <c r="A715" s="19"/>
       <c r="B715" s="19"/>
       <c r="C715" s="19" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="D715" s="56" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="E715" s="57"/>
       <c r="F715" s="9" t="s">
@@ -33346,7 +33346,7 @@
         <v>54</v>
       </c>
       <c r="K715" s="15" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="L715" s="13" t="s">
         <v>60</v>
@@ -33354,7 +33354,7 @@
       <c r="M715" s="13"/>
       <c r="N715" s="11"/>
       <c r="O715" s="11" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="P715" s="13"/>
       <c r="Q715" s="13"/>
@@ -33388,7 +33388,7 @@
         <v>221</v>
       </c>
       <c r="K716" s="15" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="L716" s="13"/>
       <c r="M716" s="13"/>
@@ -33426,7 +33426,7 @@
         <v>34</v>
       </c>
       <c r="K717" s="15" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="L717" s="13"/>
       <c r="M717" s="13"/>
@@ -33464,7 +33464,7 @@
         <v>34</v>
       </c>
       <c r="K718" s="15" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="L718" s="13"/>
       <c r="M718" s="13"/>
@@ -33502,7 +33502,7 @@
         <v>34</v>
       </c>
       <c r="K719" s="15" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="L719" s="13" t="s">
         <v>60</v>
@@ -33510,7 +33510,7 @@
       <c r="M719" s="13"/>
       <c r="N719" s="11"/>
       <c r="O719" s="11" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="P719" s="13"/>
       <c r="Q719" s="13"/>
@@ -33544,7 +33544,7 @@
         <v>34</v>
       </c>
       <c r="K720" s="15" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="L720" s="13"/>
       <c r="M720" s="13"/>
@@ -33582,7 +33582,7 @@
         <v>174</v>
       </c>
       <c r="K721" s="15" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="L721" s="13"/>
       <c r="M721" s="13"/>
@@ -33620,7 +33620,7 @@
         <v>174</v>
       </c>
       <c r="K722" s="15" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="L722" s="13"/>
       <c r="M722" s="13"/>
@@ -33658,7 +33658,7 @@
         <v>34</v>
       </c>
       <c r="K723" s="15" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="L723" s="13" t="s">
         <v>60</v>
@@ -33666,7 +33666,7 @@
       <c r="M723" s="13"/>
       <c r="N723" s="11"/>
       <c r="O723" s="11" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="P723" s="13"/>
       <c r="Q723" s="13"/>
@@ -33700,7 +33700,7 @@
         <v>34</v>
       </c>
       <c r="K724" s="15" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="L724" s="13"/>
       <c r="M724" s="13"/>
@@ -33738,7 +33738,7 @@
         <v>34</v>
       </c>
       <c r="K725" s="15" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="L725" s="13"/>
       <c r="M725" s="13"/>
@@ -33776,7 +33776,7 @@
         <v>39</v>
       </c>
       <c r="K726" s="15" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="L726" s="13"/>
       <c r="M726" s="13"/>
@@ -33814,7 +33814,7 @@
         <v>34</v>
       </c>
       <c r="K727" s="15" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="L727" s="13"/>
       <c r="M727" s="13"/>
@@ -33826,7 +33826,7 @@
       <c r="S727" s="19"/>
       <c r="T727" s="25"/>
       <c r="U727" s="25" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="V727" s="1"/>
       <c r="W727" s="1"/>
@@ -33837,13 +33837,13 @@
     <row r="728" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A728" s="9"/>
       <c r="B728" s="11" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C728" s="9" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D728" s="17" t="s">
         <v>1194</v>
-      </c>
-      <c r="D728" s="17" t="s">
-        <v>1196</v>
       </c>
       <c r="E728" s="9"/>
       <c r="F728" s="9" t="s">
@@ -33908,19 +33908,19 @@
         <v>77</v>
       </c>
       <c r="O729" s="9" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="P729" s="9" t="s">
         <v>79</v>
       </c>
       <c r="Q729" s="9" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="R729" s="13"/>
       <c r="S729" s="14"/>
       <c r="T729" s="9"/>
       <c r="U729" s="9" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="V729" s="1"/>
       <c r="W729" s="1"/>
@@ -33932,10 +33932,10 @@
       <c r="A730" s="9"/>
       <c r="B730" s="11"/>
       <c r="C730" s="9" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D730" s="9" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="E730" s="9"/>
       <c r="F730" s="9" t="s">
@@ -33968,13 +33968,13 @@
         <v>79</v>
       </c>
       <c r="Q730" s="9" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="R730" s="13"/>
       <c r="S730" s="14"/>
       <c r="T730" s="9"/>
       <c r="U730" s="9" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="V730" s="1"/>
       <c r="W730" s="1"/>
@@ -33986,10 +33986,10 @@
       <c r="A731" s="9"/>
       <c r="B731" s="11"/>
       <c r="C731" s="9" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="D731" s="9" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="E731" s="9"/>
       <c r="F731" s="9" t="s">
@@ -34022,13 +34022,13 @@
         <v>79</v>
       </c>
       <c r="Q731" s="9" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="R731" s="13"/>
       <c r="S731" s="14"/>
       <c r="T731" s="9"/>
       <c r="U731" s="9" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="V731" s="1"/>
       <c r="W731" s="1"/>
@@ -34040,10 +34040,10 @@
       <c r="A732" s="9"/>
       <c r="B732" s="11"/>
       <c r="C732" s="9" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="D732" s="9" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="E732" s="9"/>
       <c r="F732" s="9" t="s">
@@ -34076,13 +34076,13 @@
         <v>79</v>
       </c>
       <c r="Q732" s="9" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="R732" s="13"/>
       <c r="S732" s="14"/>
       <c r="T732" s="9"/>
       <c r="U732" s="9" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="V732" s="1"/>
       <c r="W732" s="1"/>
@@ -34094,10 +34094,10 @@
       <c r="A733" s="9"/>
       <c r="B733" s="11"/>
       <c r="C733" s="9" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="D733" s="9" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="E733" s="9"/>
       <c r="F733" s="9" t="s">
@@ -34130,13 +34130,13 @@
         <v>79</v>
       </c>
       <c r="Q733" s="14" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="R733" s="13"/>
       <c r="S733" s="14"/>
       <c r="T733" s="9"/>
       <c r="U733" s="9" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="V733" s="1"/>
       <c r="W733" s="1"/>
@@ -34148,10 +34148,10 @@
       <c r="A734" s="9"/>
       <c r="B734" s="11"/>
       <c r="C734" s="9" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="D734" s="9" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="E734" s="9"/>
       <c r="F734" s="9" t="s">
@@ -34184,13 +34184,13 @@
         <v>79</v>
       </c>
       <c r="Q734" s="9" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="R734" s="13"/>
       <c r="S734" s="14"/>
       <c r="T734" s="9"/>
       <c r="U734" s="9" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="V734" s="1"/>
       <c r="W734" s="1"/>
@@ -34202,10 +34202,10 @@
       <c r="A735" s="9"/>
       <c r="B735" s="11"/>
       <c r="C735" s="9" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D735" s="10" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="E735" s="9"/>
       <c r="F735" s="9" t="s">
@@ -34238,13 +34238,13 @@
         <v>79</v>
       </c>
       <c r="Q735" s="9" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="R735" s="13"/>
       <c r="S735" s="14"/>
       <c r="T735" s="9"/>
       <c r="U735" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="V735" s="1"/>
       <c r="W735" s="1"/>
@@ -34256,10 +34256,10 @@
       <c r="A736" s="9"/>
       <c r="B736" s="11"/>
       <c r="C736" s="9" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="D736" s="10" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="E736" s="9"/>
       <c r="F736" s="9" t="s">
@@ -34292,13 +34292,13 @@
         <v>79</v>
       </c>
       <c r="Q736" s="9" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="R736" s="13"/>
       <c r="S736" s="14"/>
       <c r="T736" s="9"/>
       <c r="U736" s="9" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="V736" s="1"/>
       <c r="W736" s="1"/>
@@ -34310,10 +34310,10 @@
       <c r="A737" s="9"/>
       <c r="B737" s="11"/>
       <c r="C737" s="9" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="D737" s="10" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E737" s="9"/>
       <c r="F737" s="9" t="s">
@@ -34346,13 +34346,13 @@
         <v>79</v>
       </c>
       <c r="Q737" s="9" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="R737" s="13"/>
       <c r="S737" s="14"/>
       <c r="T737" s="9"/>
       <c r="U737" s="9" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="V737" s="1"/>
       <c r="W737" s="1"/>
@@ -34364,10 +34364,10 @@
       <c r="A738" s="9"/>
       <c r="B738" s="11"/>
       <c r="C738" s="9" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="D738" s="10" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="E738" s="9"/>
       <c r="F738" s="9" t="s">
@@ -34400,13 +34400,13 @@
         <v>79</v>
       </c>
       <c r="Q738" s="9" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="R738" s="13"/>
       <c r="S738" s="14"/>
       <c r="T738" s="9"/>
       <c r="U738" s="9" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="V738" s="1"/>
       <c r="W738" s="1"/>
@@ -34418,7 +34418,7 @@
       <c r="A739" s="19"/>
       <c r="B739" s="19"/>
       <c r="C739" s="19" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="D739" s="19"/>
       <c r="E739" s="9"/>
@@ -34436,7 +34436,7 @@
         <v>34</v>
       </c>
       <c r="K739" s="24" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="L739" s="19"/>
       <c r="M739" s="19"/>
@@ -34474,7 +34474,7 @@
         <v>39</v>
       </c>
       <c r="K740" s="24" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="L740" s="19"/>
       <c r="M740" s="19"/>
@@ -34512,7 +34512,7 @@
         <v>34</v>
       </c>
       <c r="K741" s="24" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="L741" s="19"/>
       <c r="M741" s="19"/>
@@ -34550,7 +34550,7 @@
         <v>39</v>
       </c>
       <c r="K742" s="24" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="L742" s="19"/>
       <c r="M742" s="19"/>
@@ -34562,7 +34562,7 @@
       <c r="S742" s="19"/>
       <c r="T742" s="25"/>
       <c r="U742" s="25" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="V742" s="1"/>
       <c r="W742" s="1"/>
@@ -34574,10 +34574,10 @@
       <c r="A743" s="19"/>
       <c r="B743" s="19"/>
       <c r="C743" s="19" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="D743" s="19" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="E743" s="9"/>
       <c r="F743" s="9" t="s">
@@ -34594,25 +34594,25 @@
         <v>39</v>
       </c>
       <c r="K743" s="24" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="L743" s="19" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="M743" s="19"/>
       <c r="N743" s="25"/>
       <c r="O743" s="25" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="P743" s="19"/>
       <c r="Q743" s="19" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="R743" s="19"/>
       <c r="S743" s="19"/>
       <c r="T743" s="25"/>
       <c r="U743" s="25" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="V743" s="1"/>
       <c r="W743" s="1"/>
@@ -34624,10 +34624,10 @@
       <c r="A744" s="19"/>
       <c r="B744" s="19"/>
       <c r="C744" s="19" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="D744" s="19" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="E744" s="9"/>
       <c r="F744" s="9" t="s">
@@ -34644,25 +34644,25 @@
         <v>39</v>
       </c>
       <c r="K744" s="24" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="L744" s="19" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="M744" s="19"/>
       <c r="N744" s="25"/>
       <c r="O744" s="25" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="P744" s="19"/>
       <c r="Q744" s="19" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="R744" s="19"/>
       <c r="S744" s="19"/>
       <c r="T744" s="25"/>
       <c r="U744" s="25" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="V744" s="1"/>
       <c r="W744" s="1"/>
@@ -34674,10 +34674,10 @@
       <c r="A745" s="19"/>
       <c r="B745" s="19"/>
       <c r="C745" s="19" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="D745" s="19" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="E745" s="9"/>
       <c r="F745" s="9" t="s">
@@ -34694,25 +34694,25 @@
         <v>39</v>
       </c>
       <c r="K745" s="24" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="L745" s="19" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="M745" s="19"/>
       <c r="N745" s="25"/>
       <c r="O745" s="25" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="P745" s="19"/>
       <c r="Q745" s="19" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="R745" s="19"/>
       <c r="S745" s="19"/>
       <c r="T745" s="25"/>
       <c r="U745" s="25" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="V745" s="1"/>
       <c r="W745" s="1"/>
@@ -34724,10 +34724,10 @@
       <c r="A746" s="19"/>
       <c r="B746" s="19"/>
       <c r="C746" s="19" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D746" s="19" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="E746" s="9"/>
       <c r="F746" s="9" t="s">
@@ -34744,25 +34744,25 @@
         <v>39</v>
       </c>
       <c r="K746" s="24" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="L746" s="19" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="M746" s="19"/>
       <c r="N746" s="25"/>
       <c r="O746" s="25" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="P746" s="19"/>
       <c r="Q746" s="19" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="R746" s="19"/>
       <c r="S746" s="19"/>
       <c r="T746" s="25"/>
       <c r="U746" s="25" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="V746" s="1"/>
       <c r="W746" s="1"/>
@@ -34774,10 +34774,10 @@
       <c r="A747" s="19"/>
       <c r="B747" s="19"/>
       <c r="C747" s="19" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="D747" s="19" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="E747" s="9"/>
       <c r="F747" s="9" t="s">
@@ -34787,14 +34787,14 @@
         <v>216</v>
       </c>
       <c r="H747" s="23" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="I747" s="23"/>
       <c r="J747" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K747" s="24" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="L747" s="19" t="s">
         <v>60</v>
@@ -34802,17 +34802,17 @@
       <c r="M747" s="19"/>
       <c r="N747" s="25"/>
       <c r="O747" s="25" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="P747" s="19"/>
       <c r="Q747" s="19" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="R747" s="19"/>
       <c r="S747" s="19"/>
       <c r="T747" s="25"/>
       <c r="U747" s="58" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="V747" s="1"/>
       <c r="W747" s="1"/>
@@ -34824,10 +34824,10 @@
       <c r="A748" s="19"/>
       <c r="B748" s="19"/>
       <c r="C748" s="19" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="D748" s="19" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="E748" s="9"/>
       <c r="F748" s="9" t="s">
@@ -34837,30 +34837,30 @@
         <v>216</v>
       </c>
       <c r="H748" s="23" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="I748" s="23"/>
       <c r="J748" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K748" s="24" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="L748" s="19" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="M748" s="19"/>
       <c r="N748" s="25"/>
       <c r="O748" s="25"/>
       <c r="P748" s="19"/>
       <c r="Q748" s="19" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="R748" s="19"/>
       <c r="S748" s="19"/>
       <c r="T748" s="25"/>
       <c r="U748" s="58" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="V748" s="1"/>
       <c r="W748" s="1"/>
@@ -34872,10 +34872,10 @@
       <c r="A749" s="19"/>
       <c r="B749" s="19"/>
       <c r="C749" s="19" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="D749" s="19" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="E749" s="9"/>
       <c r="F749" s="9" t="s">
@@ -34885,32 +34885,32 @@
         <v>216</v>
       </c>
       <c r="H749" s="23" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="I749" s="23"/>
       <c r="J749" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K749" s="24" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="L749" s="19" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="M749" s="19"/>
       <c r="N749" s="25"/>
       <c r="O749" s="25" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="P749" s="19"/>
       <c r="Q749" s="19" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="R749" s="19"/>
       <c r="S749" s="19"/>
       <c r="T749" s="25"/>
       <c r="U749" s="25" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="V749" s="1"/>
       <c r="W749" s="1"/>
@@ -34922,10 +34922,10 @@
       <c r="A750" s="19"/>
       <c r="B750" s="19"/>
       <c r="C750" s="19" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="D750" s="19" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="E750" s="9"/>
       <c r="F750" s="9" t="s">
@@ -34935,32 +34935,32 @@
         <v>216</v>
       </c>
       <c r="H750" s="23" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="I750" s="23"/>
       <c r="J750" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K750" s="24" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="L750" s="19" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="M750" s="19"/>
       <c r="N750" s="25"/>
       <c r="O750" s="25" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="P750" s="19"/>
       <c r="Q750" s="19" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="R750" s="19"/>
       <c r="S750" s="19"/>
       <c r="T750" s="25"/>
       <c r="U750" s="25" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="V750" s="1"/>
       <c r="W750" s="1"/>
@@ -34972,10 +34972,10 @@
       <c r="A751" s="19"/>
       <c r="B751" s="19"/>
       <c r="C751" s="19" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="D751" s="19" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="E751" s="9"/>
       <c r="F751" s="9" t="s">
@@ -34985,24 +34985,24 @@
         <v>216</v>
       </c>
       <c r="H751" s="23" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="I751" s="23"/>
       <c r="J751" s="23" t="s">
         <v>39</v>
       </c>
       <c r="K751" s="24" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="L751" s="19" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="M751" s="19"/>
       <c r="N751" s="25"/>
       <c r="O751" s="25"/>
       <c r="P751" s="19"/>
       <c r="Q751" s="19" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="R751" s="19"/>
       <c r="S751" s="19"/>
@@ -35027,14 +35027,14 @@
         <v>251</v>
       </c>
       <c r="H752" s="23" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="I752" s="23"/>
       <c r="J752" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K752" s="24" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="L752" s="19"/>
       <c r="M752" s="19"/>
@@ -35065,14 +35065,14 @@
         <v>251</v>
       </c>
       <c r="H753" s="23" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="I753" s="23"/>
       <c r="J753" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K753" s="24" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="L753" s="19"/>
       <c r="M753" s="19"/>
@@ -35103,14 +35103,14 @@
         <v>251</v>
       </c>
       <c r="H754" s="23" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="I754" s="23"/>
       <c r="J754" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K754" s="24" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="L754" s="19"/>
       <c r="M754" s="19"/>
@@ -35122,7 +35122,7 @@
       <c r="S754" s="19"/>
       <c r="T754" s="25"/>
       <c r="U754" s="25" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="V754" s="1"/>
       <c r="W754" s="1"/>

</xml_diff>

<commit_message>
videos to additional items
</commit_message>
<xml_diff>
--- a/VivelDialog.xlsx
+++ b/VivelDialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerja\Github\viveljs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6064AFA7-683F-4E16-A806-E35F2EFAD27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96581FDC-A725-4498-B9FA-61A87003D296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4551,10 +4551,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O607" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I514" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R528" sqref="R528"/>
+      <selection pane="bottomRight" activeCell="O525" sqref="O525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25239,10 +25239,10 @@
         <v>916</v>
       </c>
       <c r="M526" s="19"/>
-      <c r="N526" s="25"/>
-      <c r="O526" s="25" t="s">
+      <c r="N526" s="25" t="s">
         <v>917</v>
       </c>
+      <c r="O526" s="25"/>
       <c r="P526" s="19"/>
       <c r="Q526" s="19"/>
       <c r="R526" s="14"/>
@@ -27059,10 +27059,10 @@
         <v>916</v>
       </c>
       <c r="M572" s="19"/>
-      <c r="N572" s="25"/>
-      <c r="O572" s="25" t="s">
+      <c r="N572" s="25" t="s">
         <v>991</v>
       </c>
+      <c r="O572" s="25"/>
       <c r="P572" s="19"/>
       <c r="Q572" s="19"/>
       <c r="R572" s="14"/>

</xml_diff>